<commit_message>
refactor; put sql in sep file
</commit_message>
<xml_diff>
--- a/backtest_portfolio_PL.xlsx
+++ b/backtest_portfolio_PL.xlsx
@@ -12,6 +12,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025-10-24_PnL" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025-10-27_Allocations" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025-10-27_PnL" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025-10-28_Allocations" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025-10-28_PnL" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -10922,4 +10924,4682 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E105"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Allocation_Percent</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Entry_Price</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Target_Value</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Actual_Shares</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>KDP</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.04020818056104079</v>
+      </c>
+      <c r="C2" t="n">
+        <v>29.22999954223633</v>
+      </c>
+      <c r="D2" t="n">
+        <v>4939.573247802832</v>
+      </c>
+      <c r="E2" t="n">
+        <v>168.9898503304908</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.03699170257737974</v>
+      </c>
+      <c r="C3" t="n">
+        <v>527.0700073242188</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4544.429066232145</v>
+      </c>
+      <c r="E3" t="n">
+        <v>8.622059694314405</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.03144947619076791</v>
+      </c>
+      <c r="C4" t="n">
+        <v>13.26000022888184</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3863.566793665138</v>
+      </c>
+      <c r="E4" t="n">
+        <v>291.3700397417668</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>GLW</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.02977911455044821</v>
+      </c>
+      <c r="C5" t="n">
+        <v>89.37000274658203</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3658.36293819216</v>
+      </c>
+      <c r="E5" t="n">
+        <v>40.93502098870725</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ES</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.02927841242864678</v>
+      </c>
+      <c r="C6" t="n">
+        <v>74.70999908447266</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3596.851704123417</v>
+      </c>
+      <c r="E6" t="n">
+        <v>48.14418080846917</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MU</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.02604182738691457</v>
+      </c>
+      <c r="C7" t="n">
+        <v>220.1000061035156</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3199.237371335875</v>
+      </c>
+      <c r="E7" t="n">
+        <v>14.53538065706021</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>NEE</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.02402653838389583</v>
+      </c>
+      <c r="C8" t="n">
+        <v>86.02999877929688</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2951.65920423154</v>
+      </c>
+      <c r="E8" t="n">
+        <v>34.30965065806623</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.02360596933929827</v>
+      </c>
+      <c r="C9" t="n">
+        <v>269.9299926757812</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2899.992315241269</v>
+      </c>
+      <c r="E9" t="n">
+        <v>10.74349792142036</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.02220262472437933</v>
+      </c>
+      <c r="C10" t="n">
+        <v>269.2699890136719</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2727.591489822712</v>
+      </c>
+      <c r="E10" t="n">
+        <v>10.12957849411218</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>LRCX</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.02180000765177594</v>
+      </c>
+      <c r="C11" t="n">
+        <v>156.8999938964844</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2678.129999817682</v>
+      </c>
+      <c r="E11" t="n">
+        <v>17.06902551943114</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>WST</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.02145014928924827</v>
+      </c>
+      <c r="C12" t="n">
+        <v>287.2200012207031</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2635.149915070046</v>
+      </c>
+      <c r="E12" t="n">
+        <v>9.174674130877001</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>EXC</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.02130739172327973</v>
+      </c>
+      <c r="C13" t="n">
+        <v>48.06999969482422</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2617.612154247739</v>
+      </c>
+      <c r="E13" t="n">
+        <v>54.4541745551453</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>WDC</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.02116076158769948</v>
+      </c>
+      <c r="C14" t="n">
+        <v>126.6699981689453</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2599.598648415653</v>
+      </c>
+      <c r="E14" t="n">
+        <v>20.52260745238549</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>MCK</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.02081535326012632</v>
+      </c>
+      <c r="C15" t="n">
+        <v>811.4400024414062</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2557.165250270254</v>
+      </c>
+      <c r="E15" t="n">
+        <v>3.151391652588518</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ALB</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.02073848347931497</v>
+      </c>
+      <c r="C16" t="n">
+        <v>96.23000335693359</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2547.721801012864</v>
+      </c>
+      <c r="E16" t="n">
+        <v>26.47533733905138</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>SRE</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.01916403375377504</v>
+      </c>
+      <c r="C17" t="n">
+        <v>93.16999816894531</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2354.300720134036</v>
+      </c>
+      <c r="E17" t="n">
+        <v>25.2688715938899</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>STX</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.0178424365123029</v>
+      </c>
+      <c r="C18" t="n">
+        <v>230.3200073242188</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2191.942556017774</v>
+      </c>
+      <c r="E18" t="n">
+        <v>9.516943757874245</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>AMAT</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.01736709183933136</v>
+      </c>
+      <c r="C19" t="n">
+        <v>231.3300018310547</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2133.546483444152</v>
+      </c>
+      <c r="E19" t="n">
+        <v>9.222956238085914</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>CRWD</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.01556115476645614</v>
+      </c>
+      <c r="C20" t="n">
+        <v>529.7000122070312</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1911.687191928901</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3.608999712806737</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.01543110679019397</v>
+      </c>
+      <c r="C21" t="n">
+        <v>313.0899963378906</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1895.710803653875</v>
+      </c>
+      <c r="E21" t="n">
+        <v>6.054843098876914</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>BG</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.01522798894460948</v>
+      </c>
+      <c r="C22" t="n">
+        <v>96.41999816894531</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1870.757785084002</v>
+      </c>
+      <c r="E22" t="n">
+        <v>19.40217611087376</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>CVS</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.01516827196578593</v>
+      </c>
+      <c r="C23" t="n">
+        <v>82.44999694824219</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1863.421556811036</v>
+      </c>
+      <c r="E23" t="n">
+        <v>22.60062614654546</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.01494303082228358</v>
+      </c>
+      <c r="C24" t="n">
+        <v>146.5899963378906</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1835.7506920461</v>
+      </c>
+      <c r="E24" t="n">
+        <v>12.52302843240876</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>INTC</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.01487721323564412</v>
+      </c>
+      <c r="C25" t="n">
+        <v>39.54000091552734</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1827.66500436606</v>
+      </c>
+      <c r="E25" t="n">
+        <v>46.22319074475126</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>COR</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.01476750784005551</v>
+      </c>
+      <c r="C26" t="n">
+        <v>336.0499877929688</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1814.187701249435</v>
+      </c>
+      <c r="E26" t="n">
+        <v>5.398564996726341</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>KLAC</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.01456943352338175</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1215.130004882812</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1789.854279988724</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1.472973486619926</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>JBHT</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.01403818065852259</v>
+      </c>
+      <c r="C28" t="n">
+        <v>167.7700042724609</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1724.589888452948</v>
+      </c>
+      <c r="E28" t="n">
+        <v>10.2794888510117</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.01399696965600965</v>
+      </c>
+      <c r="C29" t="n">
+        <v>259.6700134277344</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1719.527118571606</v>
+      </c>
+      <c r="E29" t="n">
+        <v>6.621970307134236</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>TGT</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.0134102813004168</v>
+      </c>
+      <c r="C30" t="n">
+        <v>97.76999664306641</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1647.452479390048</v>
+      </c>
+      <c r="E30" t="n">
+        <v>16.85028675417144</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>DELL</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0.01244139823227411</v>
+      </c>
+      <c r="C31" t="n">
+        <v>162.1900024414062</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1528.425236255253</v>
+      </c>
+      <c r="E31" t="n">
+        <v>9.423671084827943</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>CEG</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0.01235739838632038</v>
+      </c>
+      <c r="C32" t="n">
+        <v>391.1499938964844</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1518.10585880263</v>
+      </c>
+      <c r="E32" t="n">
+        <v>3.881134813987466</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>PWR</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.01224588098496259</v>
+      </c>
+      <c r="C33" t="n">
+        <v>441.8200073242188</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1504.405950855411</v>
+      </c>
+      <c r="E33" t="n">
+        <v>3.405019976271557</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>DHR</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.01158792961781742</v>
+      </c>
+      <c r="C34" t="n">
+        <v>221.0099945068359</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1423.576653778124</v>
+      </c>
+      <c r="E34" t="n">
+        <v>6.441232021903388</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>HWM</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.01125452049079201</v>
+      </c>
+      <c r="C35" t="n">
+        <v>201.8399963378906</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1382.617356902508</v>
+      </c>
+      <c r="E35" t="n">
+        <v>6.850066299981173</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>MPC</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0.01119513372031912</v>
+      </c>
+      <c r="C36" t="n">
+        <v>196.2299957275391</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1375.32169471118</v>
+      </c>
+      <c r="E36" t="n">
+        <v>7.008723052824112</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>AVY</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0.01091195488835044</v>
+      </c>
+      <c r="C37" t="n">
+        <v>180.4700012207031</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1340.533187416923</v>
+      </c>
+      <c r="E37" t="n">
+        <v>7.428011183850649</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>APH</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0.01067851274023258</v>
+      </c>
+      <c r="C38" t="n">
+        <v>135.9100036621094</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1311.854829588669</v>
+      </c>
+      <c r="E38" t="n">
+        <v>9.652378737698493</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>RL</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0.01052807678364361</v>
+      </c>
+      <c r="C39" t="n">
+        <v>337.5700073242188</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1293.373778809799</v>
+      </c>
+      <c r="E39" t="n">
+        <v>3.831423855045214</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>LW</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0.01050573026912814</v>
+      </c>
+      <c r="C40" t="n">
+        <v>66.56999969482422</v>
+      </c>
+      <c r="D40" t="n">
+        <v>1290.628510465348</v>
+      </c>
+      <c r="E40" t="n">
+        <v>19.38753967826282</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0.01039341823895537</v>
+      </c>
+      <c r="C41" t="n">
+        <v>268.8099975585938</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1276.830982402479</v>
+      </c>
+      <c r="E41" t="n">
+        <v>4.749938596030687</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0.01010872867784686</v>
+      </c>
+      <c r="C42" t="n">
+        <v>351.75</v>
+      </c>
+      <c r="D42" t="n">
+        <v>1241.85688209855</v>
+      </c>
+      <c r="E42" t="n">
+        <v>3.530509970429423</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>TECH</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0.009798516248532771</v>
+      </c>
+      <c r="C43" t="n">
+        <v>64.25</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1203.747298536331</v>
+      </c>
+      <c r="E43" t="n">
+        <v>18.73536651418413</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>APP</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0.009025874080746885</v>
+      </c>
+      <c r="C44" t="n">
+        <v>643.0999755859375</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1108.82824154678</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1.724192635113244</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>IRM</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0.008592591436386052</v>
+      </c>
+      <c r="C45" t="n">
+        <v>106.4599990844727</v>
+      </c>
+      <c r="D45" t="n">
+        <v>1055.59948737391</v>
+      </c>
+      <c r="E45" t="n">
+        <v>9.915456476158006</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>WBD</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0.008505130656886413</v>
+      </c>
+      <c r="C46" t="n">
+        <v>21.04000091552734</v>
+      </c>
+      <c r="D46" t="n">
+        <v>1044.854934384437</v>
+      </c>
+      <c r="E46" t="n">
+        <v>49.66040346573097</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>TMO</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0.00848660933045137</v>
+      </c>
+      <c r="C47" t="n">
+        <v>563.780029296875</v>
+      </c>
+      <c r="D47" t="n">
+        <v>1042.57959023069</v>
+      </c>
+      <c r="E47" t="n">
+        <v>1.849266621825813</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>TER</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0.008366228458142166</v>
+      </c>
+      <c r="C48" t="n">
+        <v>147.5</v>
+      </c>
+      <c r="D48" t="n">
+        <v>1027.790805259358</v>
+      </c>
+      <c r="E48" t="n">
+        <v>6.968073255995649</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>VLO</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0.00813286338781887</v>
+      </c>
+      <c r="C49" t="n">
+        <v>174.3500061035156</v>
+      </c>
+      <c r="D49" t="n">
+        <v>999.1219164348413</v>
+      </c>
+      <c r="E49" t="n">
+        <v>5.730552804464139</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>RVTY</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>0.007938494680745029</v>
+      </c>
+      <c r="C50" t="n">
+        <v>97.16000366210938</v>
+      </c>
+      <c r="D50" t="n">
+        <v>975.2437291536628</v>
+      </c>
+      <c r="E50" t="n">
+        <v>10.03750198018971</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>DDOG</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>0.007574292223989477</v>
+      </c>
+      <c r="C51" t="n">
+        <v>157.6199951171875</v>
+      </c>
+      <c r="D51" t="n">
+        <v>930.5014730487717</v>
+      </c>
+      <c r="E51" t="n">
+        <v>5.903448178366973</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>MPWR</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>0.00734190414239466</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1105.050048828125</v>
+      </c>
+      <c r="D52" t="n">
+        <v>901.9526072474124</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.8162097347571797</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>MNST</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>0.00717505138731106</v>
+      </c>
+      <c r="C53" t="n">
+        <v>69.68000030517578</v>
+      </c>
+      <c r="D53" t="n">
+        <v>881.4547534815116</v>
+      </c>
+      <c r="E53" t="n">
+        <v>12.65003946069211</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>0.006961546419545933</v>
+      </c>
+      <c r="C54" t="n">
+        <v>172.5899963378906</v>
+      </c>
+      <c r="D54" t="n">
+        <v>855.2256773997281</v>
+      </c>
+      <c r="E54" t="n">
+        <v>4.955244774009945</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>LVS</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0.006757588433656873</v>
+      </c>
+      <c r="C55" t="n">
+        <v>59.43999862670898</v>
+      </c>
+      <c r="D55" t="n">
+        <v>830.1694476296717</v>
+      </c>
+      <c r="E55" t="n">
+        <v>13.96651189114665</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>0.006539158556114822</v>
+      </c>
+      <c r="C56" t="n">
+        <v>452.4200134277344</v>
+      </c>
+      <c r="D56" t="n">
+        <v>803.3353465941975</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1.77564060552444</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>HOOD</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>0.006473811695690953</v>
+      </c>
+      <c r="C57" t="n">
+        <v>145.8600006103516</v>
+      </c>
+      <c r="D57" t="n">
+        <v>795.3074876094413</v>
+      </c>
+      <c r="E57" t="n">
+        <v>5.452539999187406</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>CRL</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>0.006175988794448524</v>
+      </c>
+      <c r="C58" t="n">
+        <v>195.2799987792969</v>
+      </c>
+      <c r="D58" t="n">
+        <v>758.7199570364825</v>
+      </c>
+      <c r="E58" t="n">
+        <v>3.885292717017982</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>AVGO</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>0.006161823394781034</v>
+      </c>
+      <c r="C59" t="n">
+        <v>362.0499877929688</v>
+      </c>
+      <c r="D59" t="n">
+        <v>756.9797382982646</v>
+      </c>
+      <c r="E59" t="n">
+        <v>2.090815533271413</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>PANW</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>0.006103752050067547</v>
+      </c>
+      <c r="C60" t="n">
+        <v>220.2899932861328</v>
+      </c>
+      <c r="D60" t="n">
+        <v>749.8456761047464</v>
+      </c>
+      <c r="E60" t="n">
+        <v>3.403902578229135</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>FICO</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>0.005771743727202069</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1685.089965820312</v>
+      </c>
+      <c r="D61" t="n">
+        <v>709.0584679597641</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.4207837458782742</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>PCG</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>0.005756343885729223</v>
+      </c>
+      <c r="C62" t="n">
+        <v>16.43000030517578</v>
+      </c>
+      <c r="D62" t="n">
+        <v>707.1665980989981</v>
+      </c>
+      <c r="E62" t="n">
+        <v>43.04117985172687</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>UHS</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>0.005586486414523865</v>
+      </c>
+      <c r="C63" t="n">
+        <v>214.0299987792969</v>
+      </c>
+      <c r="D63" t="n">
+        <v>686.2996150871284</v>
+      </c>
+      <c r="E63" t="n">
+        <v>3.206558047943671</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>HAL</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>0.005427581909854098</v>
+      </c>
+      <c r="C64" t="n">
+        <v>26.79999923706055</v>
+      </c>
+      <c r="D64" t="n">
+        <v>666.7782035417704</v>
+      </c>
+      <c r="E64" t="n">
+        <v>24.87978442252013</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>HOLX</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>0.00533043297098047</v>
+      </c>
+      <c r="C65" t="n">
+        <v>73.94999694824219</v>
+      </c>
+      <c r="D65" t="n">
+        <v>654.8434605910393</v>
+      </c>
+      <c r="E65" t="n">
+        <v>8.855219575591951</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>EIX</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0.0053064565475773</v>
+      </c>
+      <c r="C66" t="n">
+        <v>56.90999984741211</v>
+      </c>
+      <c r="D66" t="n">
+        <v>651.8979580100284</v>
+      </c>
+      <c r="E66" t="n">
+        <v>11.45489298467592</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>IQV</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0.004799519907067081</v>
+      </c>
+      <c r="C67" t="n">
+        <v>217.4299926757812</v>
+      </c>
+      <c r="D67" t="n">
+        <v>589.6208135867967</v>
+      </c>
+      <c r="E67" t="n">
+        <v>2.711773138244108</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>IBKR</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>0.00416271397814654</v>
+      </c>
+      <c r="C68" t="n">
+        <v>69.48999786376953</v>
+      </c>
+      <c r="D68" t="n">
+        <v>511.3892326834325</v>
+      </c>
+      <c r="E68" t="n">
+        <v>7.359177556545283</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>TEL</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>0.004017244901179865</v>
+      </c>
+      <c r="C69" t="n">
+        <v>236.7400054931641</v>
+      </c>
+      <c r="D69" t="n">
+        <v>493.5183628519486</v>
+      </c>
+      <c r="E69" t="n">
+        <v>2.08464286305932</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>PLTR</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>0.003921073186576856</v>
+      </c>
+      <c r="C70" t="n">
+        <v>189.1799926757812</v>
+      </c>
+      <c r="D70" t="n">
+        <v>481.7036718607168</v>
+      </c>
+      <c r="E70" t="n">
+        <v>2.546271754467534</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>EA</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>0.003881152950818273</v>
+      </c>
+      <c r="C71" t="n">
+        <v>200.5</v>
+      </c>
+      <c r="D71" t="n">
+        <v>476.7994726194772</v>
+      </c>
+      <c r="E71" t="n">
+        <v>2.378052232516096</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>DLTR</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>0.003843855260646561</v>
+      </c>
+      <c r="C72" t="n">
+        <v>102.5899963378906</v>
+      </c>
+      <c r="D72" t="n">
+        <v>472.2174529904783</v>
+      </c>
+      <c r="E72" t="n">
+        <v>4.602958084092156</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>DOW</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>0.003792737082996114</v>
+      </c>
+      <c r="C73" t="n">
+        <v>25.72999954223633</v>
+      </c>
+      <c r="D73" t="n">
+        <v>465.9375870707743</v>
+      </c>
+      <c r="E73" t="n">
+        <v>18.10872892966547</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>EBAY</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>0.003575965864842386</v>
+      </c>
+      <c r="C74" t="n">
+        <v>98.01000213623047</v>
+      </c>
+      <c r="D74" t="n">
+        <v>439.3072522696198</v>
+      </c>
+      <c r="E74" t="n">
+        <v>4.482269591821844</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>ETR</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>0.003565955923113377</v>
+      </c>
+      <c r="C75" t="n">
+        <v>97.36000061035156</v>
+      </c>
+      <c r="D75" t="n">
+        <v>438.0775313599255</v>
+      </c>
+      <c r="E75" t="n">
+        <v>4.499563769654989</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>PLD</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>0.003424816566738904</v>
+      </c>
+      <c r="C76" t="n">
+        <v>127.0800018310547</v>
+      </c>
+      <c r="D76" t="n">
+        <v>420.738567516459</v>
+      </c>
+      <c r="E76" t="n">
+        <v>3.310816504990344</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>EL</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>0.003417530089413494</v>
+      </c>
+      <c r="C77" t="n">
+        <v>100.4599990844727</v>
+      </c>
+      <c r="D77" t="n">
+        <v>419.8434240912877</v>
+      </c>
+      <c r="E77" t="n">
+        <v>4.179209913572254</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>BIIB</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>0.003041140225678993</v>
+      </c>
+      <c r="C78" t="n">
+        <v>150.4299926757812</v>
+      </c>
+      <c r="D78" t="n">
+        <v>373.603945564658</v>
+      </c>
+      <c r="E78" t="n">
+        <v>2.483573514291655</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>UNH</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>0.003010902022918742</v>
+      </c>
+      <c r="C79" t="n">
+        <v>365.9800109863281</v>
+      </c>
+      <c r="D79" t="n">
+        <v>369.8891836596914</v>
+      </c>
+      <c r="E79" t="n">
+        <v>1.010681383015504</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>EPAM</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>0.002984209961902182</v>
+      </c>
+      <c r="C80" t="n">
+        <v>162.4499969482422</v>
+      </c>
+      <c r="D80" t="n">
+        <v>366.6100651149972</v>
+      </c>
+      <c r="E80" t="n">
+        <v>2.256756368126015</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>FSLR</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>0.002902159691958224</v>
+      </c>
+      <c r="C81" t="n">
+        <v>247.6900024414062</v>
+      </c>
+      <c r="D81" t="n">
+        <v>356.5301929910922</v>
+      </c>
+      <c r="E81" t="n">
+        <v>1.439421008021643</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>LLY</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>0.002873854897504302</v>
+      </c>
+      <c r="C82" t="n">
+        <v>826.4099731445312</v>
+      </c>
+      <c r="D82" t="n">
+        <v>353.0529502131729</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.4272128382838711</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>SMCI</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>0.00281819383098073</v>
+      </c>
+      <c r="C83" t="n">
+        <v>51.56999969482422</v>
+      </c>
+      <c r="D83" t="n">
+        <v>346.214990591334</v>
+      </c>
+      <c r="E83" t="n">
+        <v>6.713496076015714</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>MRK</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>0.002704927755747278</v>
+      </c>
+      <c r="C84" t="n">
+        <v>88</v>
+      </c>
+      <c r="D84" t="n">
+        <v>332.3002581339073</v>
+      </c>
+      <c r="E84" t="n">
+        <v>3.77613929697622</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>CSX</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>0.002701196382192164</v>
+      </c>
+      <c r="C85" t="n">
+        <v>36</v>
+      </c>
+      <c r="D85" t="n">
+        <v>331.8418590535904</v>
+      </c>
+      <c r="E85" t="n">
+        <v>9.217829418155288</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>0.002558722426686623</v>
+      </c>
+      <c r="C86" t="n">
+        <v>312.8399963378906</v>
+      </c>
+      <c r="D86" t="n">
+        <v>314.3389397644315</v>
+      </c>
+      <c r="E86" t="n">
+        <v>1.004791405971383</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>PEP</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>0.002432837716225912</v>
+      </c>
+      <c r="C87" t="n">
+        <v>152.6300048828125</v>
+      </c>
+      <c r="D87" t="n">
+        <v>298.8740085135598</v>
+      </c>
+      <c r="E87" t="n">
+        <v>1.958160249965475</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>0.002398921229679384</v>
+      </c>
+      <c r="C88" t="n">
+        <v>361.4299926757812</v>
+      </c>
+      <c r="D88" t="n">
+        <v>294.7073696040882</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0.8153926779077623</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>J</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>0.002341058248556187</v>
+      </c>
+      <c r="C89" t="n">
+        <v>161</v>
+      </c>
+      <c r="D89" t="n">
+        <v>287.5989048686507</v>
+      </c>
+      <c r="E89" t="n">
+        <v>1.786328601668638</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>BBY</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>0.002050062794829059</v>
+      </c>
+      <c r="C90" t="n">
+        <v>82.87999725341797</v>
+      </c>
+      <c r="D90" t="n">
+        <v>251.8501259284885</v>
+      </c>
+      <c r="E90" t="n">
+        <v>3.038732315089479</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>MTD</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>0.002049343158034631</v>
+      </c>
+      <c r="C91" t="n">
+        <v>1419.7099609375</v>
+      </c>
+      <c r="D91" t="n">
+        <v>251.76171857933</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0.1773332057296267</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>ANET</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>0.001666925177712811</v>
+      </c>
+      <c r="C92" t="n">
+        <v>156.8099975585938</v>
+      </c>
+      <c r="D92" t="n">
+        <v>204.7816861899321</v>
+      </c>
+      <c r="E92" t="n">
+        <v>1.305922386188503</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>0.001598056654367175</v>
+      </c>
+      <c r="C93" t="n">
+        <v>52.68000030517578</v>
+      </c>
+      <c r="D93" t="n">
+        <v>196.3211910671212</v>
+      </c>
+      <c r="E93" t="n">
+        <v>3.726674068523737</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>EVRG</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>0.001499571246272733</v>
+      </c>
+      <c r="C94" t="n">
+        <v>78.30999755859375</v>
+      </c>
+      <c r="D94" t="n">
+        <v>184.2222629302531</v>
+      </c>
+      <c r="E94" t="n">
+        <v>2.352474379690956</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>VRTX</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>0.001151955158845679</v>
+      </c>
+      <c r="C95" t="n">
+        <v>420.1700134277344</v>
+      </c>
+      <c r="D95" t="n">
+        <v>141.5176415820216</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0.3368104268734576</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>GNRC</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>0.001038059358002893</v>
+      </c>
+      <c r="C96" t="n">
+        <v>190.4100036621094</v>
+      </c>
+      <c r="D96" t="n">
+        <v>127.5255473606475</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0.6697418460583983</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>0.0005557356892212246</v>
+      </c>
+      <c r="C97" t="n">
+        <v>191.4900054931641</v>
+      </c>
+      <c r="D97" t="n">
+        <v>68.27210545274603</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0.3565309075892384</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>GEHC</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>0.0005116701161881563</v>
+      </c>
+      <c r="C98" t="n">
+        <v>78.34999847412109</v>
+      </c>
+      <c r="D98" t="n">
+        <v>62.85865170611842</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0.8022801905590408</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>IVZ</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>0.0004475787607457365</v>
+      </c>
+      <c r="C99" t="n">
+        <v>23.45999908447266</v>
+      </c>
+      <c r="D99" t="n">
+        <v>54.98503145418518</v>
+      </c>
+      <c r="E99" t="n">
+        <v>2.343778073315349</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>EW</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>0.0003673802839316077</v>
+      </c>
+      <c r="C100" t="n">
+        <v>80.81999969482422</v>
+      </c>
+      <c r="D100" t="n">
+        <v>45.13265203641447</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0.5584342020147868</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>TPR</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>0.0003564172724159082</v>
+      </c>
+      <c r="C101" t="n">
+        <v>114.9700012207031</v>
+      </c>
+      <c r="D101" t="n">
+        <v>43.78584654452971</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0.3808458387373228</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>AES</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>0.0003119279857211589</v>
+      </c>
+      <c r="C102" t="n">
+        <v>14.48999977111816</v>
+      </c>
+      <c r="D102" t="n">
+        <v>38.32033959283875</v>
+      </c>
+      <c r="E102" t="n">
+        <v>2.644605948802002</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>HUM</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>0.0002971661300699692</v>
+      </c>
+      <c r="C103" t="n">
+        <v>292.3399963378906</v>
+      </c>
+      <c r="D103" t="n">
+        <v>36.5068462627477</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0.1248780417324511</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>DLR</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>0.0001932479919362369</v>
+      </c>
+      <c r="C104" t="n">
+        <v>178.1399993896484</v>
+      </c>
+      <c r="D104" t="n">
+        <v>23.7405074748586</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0.1332688197833133</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>SLB</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>1.456351292947831e-05</v>
+      </c>
+      <c r="C105" t="n">
+        <v>36.15999984741211</v>
+      </c>
+      <c r="D105" t="n">
+        <v>1.789126935283033</v>
+      </c>
+      <c r="E105" t="n">
+        <v>0.04947806810931379</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G105"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Shares</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Entry_Price</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Exit_Price</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Sale_Value</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Transaction_Cost</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Gain_Loss</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>KDP</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>168.9898503304908</v>
+      </c>
+      <c r="C2" t="n">
+        <v>29.22999954223633</v>
+      </c>
+      <c r="D2" t="n">
+        <v>28.85000038146973</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4875.357246499172</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-64.21600130366005</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>8.622059694314405</v>
+      </c>
+      <c r="C3" t="n">
+        <v>527.0700073242188</v>
+      </c>
+      <c r="D3" t="n">
+        <v>524.469970703125</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4522.011395277671</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-22.41767095447358</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>291.3700397417668</v>
+      </c>
+      <c r="C4" t="n">
+        <v>13.26000022888184</v>
+      </c>
+      <c r="D4" t="n">
+        <v>13.13000011444092</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3825.688655154053</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-37.87813851108467</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>GLW</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>40.93502098870725</v>
+      </c>
+      <c r="C5" t="n">
+        <v>89.37000274658203</v>
+      </c>
+      <c r="D5" t="n">
+        <v>86.43000030517578</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3538.013876546345</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-120.3490616458153</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ES</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>48.14418080846917</v>
+      </c>
+      <c r="C6" t="n">
+        <v>74.70999908447266</v>
+      </c>
+      <c r="D6" t="n">
+        <v>74.87999725341797</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3605.036126706229</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>8.184422582812203</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MU</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>14.53538065706021</v>
+      </c>
+      <c r="C7" t="n">
+        <v>220.1000061035156</v>
+      </c>
+      <c r="D7" t="n">
+        <v>221.9100036621094</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3225.546374838385</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>26.30900350250977</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>NEE</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>34.30965065806623</v>
+      </c>
+      <c r="C8" t="n">
+        <v>86.02999877929688</v>
+      </c>
+      <c r="D8" t="n">
+        <v>83.56999969482422</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2867.257495024121</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-84.40170920741957</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>10.74349792142036</v>
+      </c>
+      <c r="C9" t="n">
+        <v>269.9299926757812</v>
+      </c>
+      <c r="D9" t="n">
+        <v>268.4299926757812</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2883.877068359138</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-16.11524688213058</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>10.12957849411218</v>
+      </c>
+      <c r="C10" t="n">
+        <v>269.2699890136719</v>
+      </c>
+      <c r="D10" t="n">
+        <v>267.4700012207031</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2709.358372185392</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-18.2331176373209</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>LRCX</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>17.06902551943114</v>
+      </c>
+      <c r="C11" t="n">
+        <v>156.8999938964844</v>
+      </c>
+      <c r="D11" t="n">
+        <v>155.6199951171875</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2656.281667989023</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-21.84833182865896</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>WST</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>9.174674130877001</v>
+      </c>
+      <c r="C12" t="n">
+        <v>287.2200012207031</v>
+      </c>
+      <c r="D12" t="n">
+        <v>283.489990234375</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2600.928279765894</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-34.22163530415173</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>EXC</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>54.4541745551453</v>
+      </c>
+      <c r="C13" t="n">
+        <v>48.06999969482422</v>
+      </c>
+      <c r="D13" t="n">
+        <v>47.70000076293945</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2597.464167825669</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>-20.14798642207052</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>WDC</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>20.52260745238549</v>
+      </c>
+      <c r="C14" t="n">
+        <v>126.6699981689453</v>
+      </c>
+      <c r="D14" t="n">
+        <v>124.9199981689453</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2563.684085373978</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>-35.91456304167468</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>MCK</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>3.151391652588518</v>
+      </c>
+      <c r="C15" t="n">
+        <v>811.4400024414062</v>
+      </c>
+      <c r="D15" t="n">
+        <v>804.5900268554688</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2535.578294388295</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>-21.5869558819586</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ALB</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>26.47533733905138</v>
+      </c>
+      <c r="C16" t="n">
+        <v>96.23000335693359</v>
+      </c>
+      <c r="D16" t="n">
+        <v>96.68000030517578</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2559.635622019119</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>11.9138210062556</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>SRE</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>25.2688715938899</v>
+      </c>
+      <c r="C17" t="n">
+        <v>93.16999816894531</v>
+      </c>
+      <c r="D17" t="n">
+        <v>92.55000305175781</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2338.634143128987</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>-15.66657700504948</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>STX</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>9.516943757874245</v>
+      </c>
+      <c r="C18" t="n">
+        <v>230.3200073242188</v>
+      </c>
+      <c r="D18" t="n">
+        <v>223</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2122.278458005957</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>-69.66409801181726</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>AMAT</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>9.222956238085914</v>
+      </c>
+      <c r="C19" t="n">
+        <v>231.3300018310547</v>
+      </c>
+      <c r="D19" t="n">
+        <v>227.6399993896484</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2099.513752408632</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>-34.0327310355201</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>CRWD</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>3.608999712806737</v>
+      </c>
+      <c r="C20" t="n">
+        <v>529.7000122070312</v>
+      </c>
+      <c r="D20" t="n">
+        <v>546.9400024414062</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1973.906311733551</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>62.21911980465029</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>IBM</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>6.054843098876914</v>
+      </c>
+      <c r="C21" t="n">
+        <v>313.0899963378906</v>
+      </c>
+      <c r="D21" t="n">
+        <v>312.5700073242188</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1892.562351762952</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>-3.14845189092307</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>BG</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>19.40217611087376</v>
+      </c>
+      <c r="C22" t="n">
+        <v>96.41999816894531</v>
+      </c>
+      <c r="D22" t="n">
+        <v>96.37000274658203</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1869.787765094572</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>-0.9700199894298294</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>CVS</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>22.60062614654546</v>
+      </c>
+      <c r="C23" t="n">
+        <v>82.44999694824219</v>
+      </c>
+      <c r="D23" t="n">
+        <v>82.19999694824219</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1857.771400274399</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>-5.650156536636359</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>12.52302843240876</v>
+      </c>
+      <c r="C24" t="n">
+        <v>146.5899963378906</v>
+      </c>
+      <c r="D24" t="n">
+        <v>145.8500061035156</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1826.483773301317</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>-9.26691874478297</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>INTC</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>46.22319074475126</v>
+      </c>
+      <c r="C25" t="n">
+        <v>39.54000091552734</v>
+      </c>
+      <c r="D25" t="n">
+        <v>41.52999877929688</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1919.649055204726</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>91.98405083866646</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>COR</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>5.398564996726341</v>
+      </c>
+      <c r="C26" t="n">
+        <v>336.0499877929688</v>
+      </c>
+      <c r="D26" t="n">
+        <v>335.6400146484375</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1811.974434581771</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>-2.213266667664357</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>KLAC</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1.472973486619926</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1215.130004882812</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1206.0400390625</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1776.465001341122</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>-13.38927864760171</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>JBHT</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>10.2794888510117</v>
+      </c>
+      <c r="C28" t="n">
+        <v>167.7700042724609</v>
+      </c>
+      <c r="D28" t="n">
+        <v>166.5599975585938</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1712.151637928101</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>-12.43825052484704</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>AMD</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>6.621970307134236</v>
+      </c>
+      <c r="C29" t="n">
+        <v>259.6700134277344</v>
+      </c>
+      <c r="D29" t="n">
+        <v>258.010009765625</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1708.534623611383</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>-10.99249496022253</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>TGT</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>16.85028675417144</v>
+      </c>
+      <c r="C30" t="n">
+        <v>97.76999664306641</v>
+      </c>
+      <c r="D30" t="n">
+        <v>97.11000061035156</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1636.331356982188</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>-11.12112240786064</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>DELL</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>9.423671084827943</v>
+      </c>
+      <c r="C31" t="n">
+        <v>162.1900024414062</v>
+      </c>
+      <c r="D31" t="n">
+        <v>164.8800048828125</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1553.77493448045</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>25.34969822519656</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>CEG</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>3.881134813987466</v>
+      </c>
+      <c r="C32" t="n">
+        <v>391.1499938964844</v>
+      </c>
+      <c r="D32" t="n">
+        <v>384.9500122070312</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1494.042894021609</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>-24.06296478102126</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>PWR</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>3.405019976271557</v>
+      </c>
+      <c r="C33" t="n">
+        <v>441.8200073242188</v>
+      </c>
+      <c r="D33" t="n">
+        <v>439.5700073242188</v>
+      </c>
+      <c r="E33" t="n">
+        <v>1496.7446559088</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>-7.661294946610951</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>DHR</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>6.441232021903388</v>
+      </c>
+      <c r="C34" t="n">
+        <v>221.0099945068359</v>
+      </c>
+      <c r="D34" t="n">
+        <v>216.8999938964844</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1397.103186236684</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>-26.47346754143905</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>HWM</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>6.850066299981173</v>
+      </c>
+      <c r="C35" t="n">
+        <v>201.8399963378906</v>
+      </c>
+      <c r="D35" t="n">
+        <v>201.0399932861328</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1377.13728295778</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>-5.480073944728247</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>MPC</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>7.008723052824112</v>
+      </c>
+      <c r="C36" t="n">
+        <v>196.2299957275391</v>
+      </c>
+      <c r="D36" t="n">
+        <v>192.2100067138672</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1347.146705038958</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>-28.17498967222173</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>AVY</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>7.428011183850649</v>
+      </c>
+      <c r="C37" t="n">
+        <v>180.4700012207031</v>
+      </c>
+      <c r="D37" t="n">
+        <v>179.1699981689453</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1330.876750209426</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>-9.656437207496992</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>APH</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>9.652378737698493</v>
+      </c>
+      <c r="C38" t="n">
+        <v>135.9100036621094</v>
+      </c>
+      <c r="D38" t="n">
+        <v>137.2899932861328</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1325.175012093837</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>13.3201825051683</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>RL</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>3.831423855045214</v>
+      </c>
+      <c r="C39" t="n">
+        <v>337.5700073242188</v>
+      </c>
+      <c r="D39" t="n">
+        <v>331.2000122070312</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1268.967627561286</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>-24.40615124851365</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>LW</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>19.38753967826282</v>
+      </c>
+      <c r="C40" t="n">
+        <v>66.56999969482422</v>
+      </c>
+      <c r="D40" t="n">
+        <v>65.56999969482422</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1271.240970787085</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>-19.38753967826278</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>4.749938596030687</v>
+      </c>
+      <c r="C41" t="n">
+        <v>268.8099975585938</v>
+      </c>
+      <c r="D41" t="n">
+        <v>269</v>
+      </c>
+      <c r="E41" t="n">
+        <v>1277.733482332255</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.9024999297755585</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>3.530509970429423</v>
+      </c>
+      <c r="C42" t="n">
+        <v>351.75</v>
+      </c>
+      <c r="D42" t="n">
+        <v>345.9500122070312</v>
+      </c>
+      <c r="E42" t="n">
+        <v>1221.379967367105</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>-20.47691473144505</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>TECH</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>18.73536651418413</v>
+      </c>
+      <c r="C43" t="n">
+        <v>64.25</v>
+      </c>
+      <c r="D43" t="n">
+        <v>63.93999862670898</v>
+      </c>
+      <c r="E43" t="n">
+        <v>1197.939309187823</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>-5.80798934850759</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>APP</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>1.724192635113244</v>
+      </c>
+      <c r="C44" t="n">
+        <v>643.0999755859375</v>
+      </c>
+      <c r="D44" t="n">
+        <v>626.8200073242188</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1080.758440170048</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>-28.06980137673281</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>IRM</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>9.915456476158006</v>
+      </c>
+      <c r="C45" t="n">
+        <v>106.4599990844727</v>
+      </c>
+      <c r="D45" t="n">
+        <v>104.0500030517578</v>
+      </c>
+      <c r="E45" t="n">
+        <v>1031.703276603812</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>-23.89621077009747</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>WBD</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>49.66040346573097</v>
+      </c>
+      <c r="C46" t="n">
+        <v>21.04000091552734</v>
+      </c>
+      <c r="D46" t="n">
+        <v>20.98999977111816</v>
+      </c>
+      <c r="E46" t="n">
+        <v>1042.371857379329</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>-2.483077005108044</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>TMO</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>1.849266621825813</v>
+      </c>
+      <c r="C47" t="n">
+        <v>563.780029296875</v>
+      </c>
+      <c r="D47" t="n">
+        <v>557.6300048828125</v>
+      </c>
+      <c r="E47" t="n">
+        <v>1031.20655535835</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>-11.37303487233953</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>TER</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>6.968073255995649</v>
+      </c>
+      <c r="C48" t="n">
+        <v>147.5</v>
+      </c>
+      <c r="D48" t="n">
+        <v>144.3800048828125</v>
+      </c>
+      <c r="E48" t="n">
+        <v>1006.050450724447</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>-21.74035453491115</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>VLO</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>5.730552804464139</v>
+      </c>
+      <c r="C49" t="n">
+        <v>174.3500061035156</v>
+      </c>
+      <c r="D49" t="n">
+        <v>169.3399963378906</v>
+      </c>
+      <c r="E49" t="n">
+        <v>970.4117909220462</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>-28.71012551279512</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>RVTY</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>10.03750198018971</v>
+      </c>
+      <c r="C50" t="n">
+        <v>97.16000366210938</v>
+      </c>
+      <c r="D50" t="n">
+        <v>96.44999694824219</v>
+      </c>
+      <c r="E50" t="n">
+        <v>968.1170353572729</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>-7.126693796389873</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>DDOG</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>5.903448178366973</v>
+      </c>
+      <c r="C51" t="n">
+        <v>157.6199951171875</v>
+      </c>
+      <c r="D51" t="n">
+        <v>157.2700042724609</v>
+      </c>
+      <c r="E51" t="n">
+        <v>928.4353202340255</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>-2.066152814746147</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>MPWR</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>0.8162097347571797</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1105.050048828125</v>
+      </c>
+      <c r="D52" t="n">
+        <v>1086.359985351562</v>
+      </c>
+      <c r="E52" t="n">
+        <v>886.6975954946125</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="n">
+        <v>-15.25501175279987</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>MNST</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>12.65003946069211</v>
+      </c>
+      <c r="C53" t="n">
+        <v>69.68000030517578</v>
+      </c>
+      <c r="D53" t="n">
+        <v>69.31999969482422</v>
+      </c>
+      <c r="E53" t="n">
+        <v>876.9007315546911</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" t="n">
+        <v>-4.554021926820496</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>4.955244774009945</v>
+      </c>
+      <c r="C54" t="n">
+        <v>172.5899963378906</v>
+      </c>
+      <c r="D54" t="n">
+        <v>172.7599945068359</v>
+      </c>
+      <c r="E54" t="n">
+        <v>856.0680599379855</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.8423825382575387</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>LVS</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>13.96651189114665</v>
+      </c>
+      <c r="C55" t="n">
+        <v>59.43999862670898</v>
+      </c>
+      <c r="D55" t="n">
+        <v>58.20000076293945</v>
+      </c>
+      <c r="E55" t="n">
+        <v>812.8510027203381</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" t="n">
+        <v>-17.31844490933361</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>1.77564060552444</v>
+      </c>
+      <c r="C56" t="n">
+        <v>452.4200134277344</v>
+      </c>
+      <c r="D56" t="n">
+        <v>460.5499877929688</v>
+      </c>
+      <c r="E56" t="n">
+        <v>817.7712591989805</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" t="n">
+        <v>14.43591260478297</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>HOOD</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>5.452539999187406</v>
+      </c>
+      <c r="C57" t="n">
+        <v>145.8600006103516</v>
+      </c>
+      <c r="D57" t="n">
+        <v>146.25</v>
+      </c>
+      <c r="E57" t="n">
+        <v>797.4339748811581</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" t="n">
+        <v>2.126487271716769</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>CRL</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>3.885292717017982</v>
+      </c>
+      <c r="C58" t="n">
+        <v>195.2799987792969</v>
+      </c>
+      <c r="D58" t="n">
+        <v>187.9299926757812</v>
+      </c>
+      <c r="E58" t="n">
+        <v>730.1630318524556</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" t="n">
+        <v>-28.55692518402691</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>AVGO</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>2.090815533271413</v>
+      </c>
+      <c r="C59" t="n">
+        <v>362.0499877929688</v>
+      </c>
+      <c r="D59" t="n">
+        <v>372.9700012207031</v>
+      </c>
+      <c r="E59" t="n">
+        <v>779.8114719965041</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" t="n">
+        <v>22.83173369823942</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>PANW</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>3.403902578229135</v>
+      </c>
+      <c r="C60" t="n">
+        <v>220.2899932861328</v>
+      </c>
+      <c r="D60" t="n">
+        <v>221.3800048828125</v>
+      </c>
+      <c r="E60" t="n">
+        <v>753.5559693889841</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" t="n">
+        <v>3.71029328423765</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>FICO</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>0.4207837458782742</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1685.089965820312</v>
+      </c>
+      <c r="D61" t="n">
+        <v>1666.640014648438</v>
+      </c>
+      <c r="E61" t="n">
+        <v>701.2950283943914</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="n">
+        <v>-7.763439565372778</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>PCG</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>43.04117985172687</v>
+      </c>
+      <c r="C62" t="n">
+        <v>16.43000030517578</v>
+      </c>
+      <c r="D62" t="n">
+        <v>16.1200008392334</v>
+      </c>
+      <c r="E62" t="n">
+        <v>693.8238553314327</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" t="n">
+        <v>-13.34274276756537</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>UHS</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>3.206558047943671</v>
+      </c>
+      <c r="C63" t="n">
+        <v>214.0299987792969</v>
+      </c>
+      <c r="D63" t="n">
+        <v>219.3200073242188</v>
+      </c>
+      <c r="E63" t="n">
+        <v>703.2623345605384</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0</v>
+      </c>
+      <c r="G63" t="n">
+        <v>16.96271947341006</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>HAL</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>24.87978442252013</v>
+      </c>
+      <c r="C64" t="n">
+        <v>26.79999923706055</v>
+      </c>
+      <c r="D64" t="n">
+        <v>26.6200008392334</v>
+      </c>
+      <c r="E64" t="n">
+        <v>662.2998822074319</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G64" t="n">
+        <v>-4.478321334338489</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>HOLX</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>8.855219575591951</v>
+      </c>
+      <c r="C65" t="n">
+        <v>73.94999694824219</v>
+      </c>
+      <c r="D65" t="n">
+        <v>74.01000213623047</v>
+      </c>
+      <c r="E65" t="n">
+        <v>655.3748197063502</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0.5313591153109201</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>EIX</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>11.45489298467592</v>
+      </c>
+      <c r="C66" t="n">
+        <v>56.90999984741211</v>
+      </c>
+      <c r="D66" t="n">
+        <v>56.04999923706055</v>
+      </c>
+      <c r="E66" t="n">
+        <v>642.0467430516953</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" t="n">
+        <v>-9.851214958333117</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>IQV</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>2.711773138244108</v>
+      </c>
+      <c r="C67" t="n">
+        <v>217.4299926757812</v>
+      </c>
+      <c r="D67" t="n">
+        <v>218.1300048828125</v>
+      </c>
+      <c r="E67" t="n">
+        <v>591.519087886267</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0</v>
+      </c>
+      <c r="G67" t="n">
+        <v>1.898274299470359</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>IBKR</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>7.359177556545283</v>
+      </c>
+      <c r="C68" t="n">
+        <v>69.48999786376953</v>
+      </c>
+      <c r="D68" t="n">
+        <v>68.65000152587891</v>
+      </c>
+      <c r="E68" t="n">
+        <v>505.2075504860475</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" t="n">
+        <v>-6.18168219738493</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>TEL</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>2.08464286305932</v>
+      </c>
+      <c r="C69" t="n">
+        <v>236.7400054931641</v>
+      </c>
+      <c r="D69" t="n">
+        <v>236.5399932861328</v>
+      </c>
+      <c r="E69" t="n">
+        <v>493.1014088320362</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0</v>
+      </c>
+      <c r="G69" t="n">
+        <v>-0.4169540199124526</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>PLTR</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>2.546271754467534</v>
+      </c>
+      <c r="C70" t="n">
+        <v>189.1799926757812</v>
+      </c>
+      <c r="D70" t="n">
+        <v>189.6000061035156</v>
+      </c>
+      <c r="E70" t="n">
+        <v>482.7731401882539</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" t="n">
+        <v>1.069468327537152</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>EA</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>2.378052232516096</v>
+      </c>
+      <c r="C71" t="n">
+        <v>200.5</v>
+      </c>
+      <c r="D71" t="n">
+        <v>200.3000030517578</v>
+      </c>
+      <c r="E71" t="n">
+        <v>476.3238694302135</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" t="n">
+        <v>-0.4756031892637225</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>DLTR</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>4.602958084092156</v>
+      </c>
+      <c r="C72" t="n">
+        <v>102.5899963378906</v>
+      </c>
+      <c r="D72" t="n">
+        <v>102.6999969482422</v>
+      </c>
+      <c r="E72" t="n">
+        <v>472.7237811891511</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0.5063281986727475</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>DOW</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>18.10872892966547</v>
+      </c>
+      <c r="C73" t="n">
+        <v>25.72999954223633</v>
+      </c>
+      <c r="D73" t="n">
+        <v>25.3799991607666</v>
+      </c>
+      <c r="E73" t="n">
+        <v>459.5995250374596</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0</v>
+      </c>
+      <c r="G73" t="n">
+        <v>-6.33806203331477</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>EBAY</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>4.482269591821844</v>
+      </c>
+      <c r="C74" t="n">
+        <v>98.01000213623047</v>
+      </c>
+      <c r="D74" t="n">
+        <v>99.58000183105469</v>
+      </c>
+      <c r="E74" t="n">
+        <v>446.3444141609</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" t="n">
+        <v>7.037161891280221</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>ETR</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>4.499563769654989</v>
+      </c>
+      <c r="C75" t="n">
+        <v>97.36000061035156</v>
+      </c>
+      <c r="D75" t="n">
+        <v>95.01999664306641</v>
+      </c>
+      <c r="E75" t="n">
+        <v>427.5485342878803</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0</v>
+      </c>
+      <c r="G75" t="n">
+        <v>-10.52899707204523</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>PLD</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>3.310816504990344</v>
+      </c>
+      <c r="C76" t="n">
+        <v>127.0800018310547</v>
+      </c>
+      <c r="D76" t="n">
+        <v>125.7200012207031</v>
+      </c>
+      <c r="E76" t="n">
+        <v>416.2358550489101</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G76" t="n">
+        <v>-4.502712467548861</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>EL</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>4.179209913572254</v>
+      </c>
+      <c r="C77" t="n">
+        <v>100.4599990844727</v>
+      </c>
+      <c r="D77" t="n">
+        <v>98.76000213623047</v>
+      </c>
+      <c r="E77" t="n">
+        <v>412.7387799921514</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0</v>
+      </c>
+      <c r="G77" t="n">
+        <v>-7.104644099136294</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>BIIB</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>2.483573514291655</v>
+      </c>
+      <c r="C78" t="n">
+        <v>150.4299926757812</v>
+      </c>
+      <c r="D78" t="n">
+        <v>149.1300048828125</v>
+      </c>
+      <c r="E78" t="n">
+        <v>370.3753303131384</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0</v>
+      </c>
+      <c r="G78" t="n">
+        <v>-3.22861525151967</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>UNH</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>1.010681383015504</v>
+      </c>
+      <c r="C79" t="n">
+        <v>365.9800109863281</v>
+      </c>
+      <c r="D79" t="n">
+        <v>367.8399963378906</v>
+      </c>
+      <c r="E79" t="n">
+        <v>371.7690362271971</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0</v>
+      </c>
+      <c r="G79" t="n">
+        <v>1.879852567505736</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>EPAM</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>2.256756368126015</v>
+      </c>
+      <c r="C80" t="n">
+        <v>162.4499969482422</v>
+      </c>
+      <c r="D80" t="n">
+        <v>161.8999938964844</v>
+      </c>
+      <c r="E80" t="n">
+        <v>365.368842225454</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0</v>
+      </c>
+      <c r="G80" t="n">
+        <v>-1.241222889543167</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>FSLR</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>1.439421008021643</v>
+      </c>
+      <c r="C81" t="n">
+        <v>247.6900024414062</v>
+      </c>
+      <c r="D81" t="n">
+        <v>239.6000061035156</v>
+      </c>
+      <c r="E81" t="n">
+        <v>344.8852823075143</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0</v>
+      </c>
+      <c r="G81" t="n">
+        <v>-11.6449106835779</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>LLY</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>0.4272128382838711</v>
+      </c>
+      <c r="C82" t="n">
+        <v>826.4099731445312</v>
+      </c>
+      <c r="D82" t="n">
+        <v>820.0999755859375</v>
+      </c>
+      <c r="E82" t="n">
+        <v>350.3572382466018</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0</v>
+      </c>
+      <c r="G82" t="n">
+        <v>-2.695711966571139</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>SMCI</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>6.713496076015714</v>
+      </c>
+      <c r="C83" t="n">
+        <v>51.56999969482422</v>
+      </c>
+      <c r="D83" t="n">
+        <v>52.36000061035156</v>
+      </c>
+      <c r="E83" t="n">
+        <v>351.5186586377756</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0</v>
+      </c>
+      <c r="G83" t="n">
+        <v>5.303668046441658</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>MRK</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>3.77613929697622</v>
+      </c>
+      <c r="C84" t="n">
+        <v>88</v>
+      </c>
+      <c r="D84" t="n">
+        <v>87.02999877929688</v>
+      </c>
+      <c r="E84" t="n">
+        <v>328.6373984062953</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" t="n">
+        <v>-3.662859727611988</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>CSX</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>9.217829418155288</v>
+      </c>
+      <c r="C85" t="n">
+        <v>36</v>
+      </c>
+      <c r="D85" t="n">
+        <v>35.68000030517578</v>
+      </c>
+      <c r="E85" t="n">
+        <v>328.892156452839</v>
+      </c>
+      <c r="F85" t="n">
+        <v>0</v>
+      </c>
+      <c r="G85" t="n">
+        <v>-2.94970260075138</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>GE</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>1.004791405971383</v>
+      </c>
+      <c r="C86" t="n">
+        <v>312.8399963378906</v>
+      </c>
+      <c r="D86" t="n">
+        <v>309.7900085449219</v>
+      </c>
+      <c r="E86" t="n">
+        <v>311.2743382417389</v>
+      </c>
+      <c r="F86" t="n">
+        <v>0</v>
+      </c>
+      <c r="G86" t="n">
+        <v>-3.064601522692612</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>PEP</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>1.958160249965475</v>
+      </c>
+      <c r="C87" t="n">
+        <v>152.6300048828125</v>
+      </c>
+      <c r="D87" t="n">
+        <v>150.1199951171875</v>
+      </c>
+      <c r="E87" t="n">
+        <v>293.9590071634878</v>
+      </c>
+      <c r="F87" t="n">
+        <v>0</v>
+      </c>
+      <c r="G87" t="n">
+        <v>-4.915001350072032</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>0.8153926779077623</v>
+      </c>
+      <c r="C88" t="n">
+        <v>361.4299926757812</v>
+      </c>
+      <c r="D88" t="n">
+        <v>355.2200012207031</v>
+      </c>
+      <c r="E88" t="n">
+        <v>289.6437880417477</v>
+      </c>
+      <c r="F88" t="n">
+        <v>0</v>
+      </c>
+      <c r="G88" t="n">
+        <v>-5.06358156234046</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>J</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>1.786328601668638</v>
+      </c>
+      <c r="C89" t="n">
+        <v>161</v>
+      </c>
+      <c r="D89" t="n">
+        <v>158.3099975585938</v>
+      </c>
+      <c r="E89" t="n">
+        <v>282.7936765690082</v>
+      </c>
+      <c r="F89" t="n">
+        <v>0</v>
+      </c>
+      <c r="G89" t="n">
+        <v>-4.805228299642465</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>BBY</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>3.038732315089479</v>
+      </c>
+      <c r="C90" t="n">
+        <v>82.87999725341797</v>
+      </c>
+      <c r="D90" t="n">
+        <v>83.86000061035156</v>
+      </c>
+      <c r="E90" t="n">
+        <v>254.8280937980988</v>
+      </c>
+      <c r="F90" t="n">
+        <v>0</v>
+      </c>
+      <c r="G90" t="n">
+        <v>2.977967869610296</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>MTD</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>0.1773332057296267</v>
+      </c>
+      <c r="C91" t="n">
+        <v>1419.7099609375</v>
+      </c>
+      <c r="D91" t="n">
+        <v>1404.579956054688</v>
+      </c>
+      <c r="E91" t="n">
+        <v>249.0786663107559</v>
+      </c>
+      <c r="F91" t="n">
+        <v>0</v>
+      </c>
+      <c r="G91" t="n">
+        <v>-2.683052268574045</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>ANET</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>1.305922386188503</v>
+      </c>
+      <c r="C92" t="n">
+        <v>156.8099975585938</v>
+      </c>
+      <c r="D92" t="n">
+        <v>156.7700042724609</v>
+      </c>
+      <c r="E92" t="n">
+        <v>204.729458062274</v>
+      </c>
+      <c r="F92" t="n">
+        <v>0</v>
+      </c>
+      <c r="G92" t="n">
+        <v>-0.05222812765808271</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>3.726674068523737</v>
+      </c>
+      <c r="C93" t="n">
+        <v>52.68000030517578</v>
+      </c>
+      <c r="D93" t="n">
+        <v>51.79999923706055</v>
+      </c>
+      <c r="E93" t="n">
+        <v>193.0417139063029</v>
+      </c>
+      <c r="F93" t="n">
+        <v>0</v>
+      </c>
+      <c r="G93" t="n">
+        <v>-3.279477160818232</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>EVRG</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>2.352474379690956</v>
+      </c>
+      <c r="C94" t="n">
+        <v>78.30999755859375</v>
+      </c>
+      <c r="D94" t="n">
+        <v>77.68000030517578</v>
+      </c>
+      <c r="E94" t="n">
+        <v>182.7402105323117</v>
+      </c>
+      <c r="F94" t="n">
+        <v>0</v>
+      </c>
+      <c r="G94" t="n">
+        <v>-1.48205239794143</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>VRTX</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>0.3368104268734576</v>
+      </c>
+      <c r="C95" t="n">
+        <v>420.1700134277344</v>
+      </c>
+      <c r="D95" t="n">
+        <v>422.3900146484375</v>
+      </c>
+      <c r="E95" t="n">
+        <v>142.2653611408262</v>
+      </c>
+      <c r="F95" t="n">
+        <v>0</v>
+      </c>
+      <c r="G95" t="n">
+        <v>0.7477195588046186</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>GNRC</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>0.6697418460583983</v>
+      </c>
+      <c r="C96" t="n">
+        <v>190.4100036621094</v>
+      </c>
+      <c r="D96" t="n">
+        <v>190.1499938964844</v>
+      </c>
+      <c r="E96" t="n">
+        <v>127.3514079402246</v>
+      </c>
+      <c r="F96" t="n">
+        <v>0</v>
+      </c>
+      <c r="G96" t="n">
+        <v>-0.1741394204229039</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>0.3565309075892384</v>
+      </c>
+      <c r="C97" t="n">
+        <v>191.4900054931641</v>
+      </c>
+      <c r="D97" t="n">
+        <v>201.0299987792969</v>
+      </c>
+      <c r="E97" t="n">
+        <v>71.6734079174462</v>
+      </c>
+      <c r="F97" t="n">
+        <v>0</v>
+      </c>
+      <c r="G97" t="n">
+        <v>3.401302464700166</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>GEHC</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>0.8022801905590408</v>
+      </c>
+      <c r="C98" t="n">
+        <v>78.34999847412109</v>
+      </c>
+      <c r="D98" t="n">
+        <v>79.40000152587891</v>
+      </c>
+      <c r="E98" t="n">
+        <v>63.70104835457025</v>
+      </c>
+      <c r="F98" t="n">
+        <v>0</v>
+      </c>
+      <c r="G98" t="n">
+        <v>0.8423966484518317</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>IVZ</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>2.343778073315349</v>
+      </c>
+      <c r="C99" t="n">
+        <v>23.45999908447266</v>
+      </c>
+      <c r="D99" t="n">
+        <v>23.95999908447266</v>
+      </c>
+      <c r="E99" t="n">
+        <v>56.15692049084286</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0</v>
+      </c>
+      <c r="G99" t="n">
+        <v>1.171889036657674</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>EW</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>0.5584342020147868</v>
+      </c>
+      <c r="C100" t="n">
+        <v>80.81999969482422</v>
+      </c>
+      <c r="D100" t="n">
+        <v>82.19000244140625</v>
+      </c>
+      <c r="E100" t="n">
+        <v>45.89770842696008</v>
+      </c>
+      <c r="F100" t="n">
+        <v>0</v>
+      </c>
+      <c r="G100" t="n">
+        <v>0.7650563905456096</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>TPR</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>0.3808458387373228</v>
+      </c>
+      <c r="C101" t="n">
+        <v>114.9700012207031</v>
+      </c>
+      <c r="D101" t="n">
+        <v>113.1100006103516</v>
+      </c>
+      <c r="E101" t="n">
+        <v>43.07747305202844</v>
+      </c>
+      <c r="F101" t="n">
+        <v>0</v>
+      </c>
+      <c r="G101" t="n">
+        <v>-0.7083734925012735</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>AES</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>2.644605948802002</v>
+      </c>
+      <c r="C102" t="n">
+        <v>14.48999977111816</v>
+      </c>
+      <c r="D102" t="n">
+        <v>14.46000003814697</v>
+      </c>
+      <c r="E102" t="n">
+        <v>38.24100212056067</v>
+      </c>
+      <c r="F102" t="n">
+        <v>0</v>
+      </c>
+      <c r="G102" t="n">
+        <v>-0.07933747227808396</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>HUM</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>0.1248780417324511</v>
+      </c>
+      <c r="C103" t="n">
+        <v>292.3399963378906</v>
+      </c>
+      <c r="D103" t="n">
+        <v>294.7999877929688</v>
+      </c>
+      <c r="E103" t="n">
+        <v>36.81404517833642</v>
+      </c>
+      <c r="F103" t="n">
+        <v>0</v>
+      </c>
+      <c r="G103" t="n">
+        <v>0.3071989155887209</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>DLR</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>0.1332688197833133</v>
+      </c>
+      <c r="C104" t="n">
+        <v>178.1399993896484</v>
+      </c>
+      <c r="D104" t="n">
+        <v>174.0599975585938</v>
+      </c>
+      <c r="E104" t="n">
+        <v>23.19677044612019</v>
+      </c>
+      <c r="F104" t="n">
+        <v>0</v>
+      </c>
+      <c r="G104" t="n">
+        <v>-0.5437370287384127</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>SLB</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>0.04947806810931379</v>
+      </c>
+      <c r="C105" t="n">
+        <v>36.15999984741211</v>
+      </c>
+      <c r="D105" t="n">
+        <v>35.86000061035156</v>
+      </c>
+      <c r="E105" t="n">
+        <v>1.774283552599009</v>
+      </c>
+      <c r="F105" t="n">
+        <v>0</v>
+      </c>
+      <c r="G105" t="n">
+        <v>-0.01484338268402396</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new chnages overriding old
</commit_message>
<xml_diff>
--- a/backtest_portfolio_PL.xlsx
+++ b/backtest_portfolio_PL.xlsx
@@ -28,6 +28,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025-11-06_Allocations" sheetId="20" state="visible" r:id="rId20"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025-11-05_PnL" sheetId="21" state="visible" r:id="rId21"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025-11-06_PnL" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025-11-07_Allocations" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2025-11-07_PnL" sheetId="24" state="visible" r:id="rId24"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -30345,6 +30347,3804 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E85"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Allocation_Percent</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Entry_Price</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Target_Value</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Actual_Shares</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>LRCX</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.07932298484724096</v>
+      </c>
+      <c r="C2" t="n">
+        <v>162.1900024414062</v>
+      </c>
+      <c r="D2" t="n">
+        <v>9569.783944975063</v>
+      </c>
+      <c r="E2" t="n">
+        <v>59.00353783170021</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>AMAT</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.07603565413088466</v>
+      </c>
+      <c r="C3" t="n">
+        <v>233.5299987792969</v>
+      </c>
+      <c r="D3" t="n">
+        <v>9173.189631589185</v>
+      </c>
+      <c r="E3" t="n">
+        <v>39.28056215278161</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>BIIB</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.05777423973410276</v>
+      </c>
+      <c r="C4" t="n">
+        <v>156.7400054931641</v>
+      </c>
+      <c r="D4" t="n">
+        <v>6970.072960634279</v>
+      </c>
+      <c r="E4" t="n">
+        <v>44.46901056755588</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>HOOD</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.05367543781681008</v>
+      </c>
+      <c r="C5" t="n">
+        <v>127.0800018310547</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6475.580111464789</v>
+      </c>
+      <c r="E5" t="n">
+        <v>50.95672031917098</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>TEL</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.04124713959308426</v>
+      </c>
+      <c r="C6" t="n">
+        <v>242.5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4976.189625418168</v>
+      </c>
+      <c r="E6" t="n">
+        <v>20.52036958935327</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.04094277542387142</v>
+      </c>
+      <c r="C7" t="n">
+        <v>243.0399932861328</v>
+      </c>
+      <c r="D7" t="n">
+        <v>4939.470138051828</v>
+      </c>
+      <c r="E7" t="n">
+        <v>20.32369270285715</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>CSCO</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.0376588710060428</v>
+      </c>
+      <c r="C8" t="n">
+        <v>71.04000091552734</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4543.289184509935</v>
+      </c>
+      <c r="E8" t="n">
+        <v>63.95395729108021</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>CEG</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.02838121864529531</v>
+      </c>
+      <c r="C9" t="n">
+        <v>351.2999877929688</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3424.002904752278</v>
+      </c>
+      <c r="E9" t="n">
+        <v>9.746663887646196</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ISRG</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.02652111834191165</v>
+      </c>
+      <c r="C10" t="n">
+        <v>547.780029296875</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3199.594329436502</v>
+      </c>
+      <c r="E10" t="n">
+        <v>5.841020406573547</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>EXE</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.02623679059447917</v>
+      </c>
+      <c r="C11" t="n">
+        <v>110.620002746582</v>
+      </c>
+      <c r="D11" t="n">
+        <v>3165.29210142869</v>
+      </c>
+      <c r="E11" t="n">
+        <v>28.61410253876072</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>EL</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.02620143993861553</v>
+      </c>
+      <c r="C12" t="n">
+        <v>87.77999877929688</v>
+      </c>
+      <c r="D12" t="n">
+        <v>3161.027282857129</v>
+      </c>
+      <c r="E12" t="n">
+        <v>36.01079205759416</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.02410465021873586</v>
+      </c>
+      <c r="C13" t="n">
+        <v>371.1600036621094</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2908.063723354978</v>
+      </c>
+      <c r="E13" t="n">
+        <v>7.83506761144009</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.02346324739518281</v>
+      </c>
+      <c r="C14" t="n">
+        <v>68.83999633789062</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2830.682792028197</v>
+      </c>
+      <c r="E14" t="n">
+        <v>41.11974059577549</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>GL</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.02235746075466328</v>
+      </c>
+      <c r="C15" t="n">
+        <v>131.8300018310547</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2697.277080437911</v>
+      </c>
+      <c r="E15" t="n">
+        <v>20.46026733652463</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>FSLR</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.0171095492070544</v>
+      </c>
+      <c r="C16" t="n">
+        <v>271.9800109863281</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2064.151892704843</v>
+      </c>
+      <c r="E16" t="n">
+        <v>7.589351457187063</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>DLTR</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.01645211583538099</v>
+      </c>
+      <c r="C17" t="n">
+        <v>101.9700012207031</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1984.836983700257</v>
+      </c>
+      <c r="E17" t="n">
+        <v>19.46491085553966</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>GLW</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.01640701427047315</v>
+      </c>
+      <c r="C18" t="n">
+        <v>87.86000061035156</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1979.395783617085</v>
+      </c>
+      <c r="E18" t="n">
+        <v>22.52897530009663</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>CVS</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.01581036187815402</v>
+      </c>
+      <c r="C19" t="n">
+        <v>78.66000366210938</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1907.413690460323</v>
+      </c>
+      <c r="E19" t="n">
+        <v>24.24883805820526</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.01446769364626673</v>
+      </c>
+      <c r="C20" t="n">
+        <v>60.5</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1745.429810079528</v>
+      </c>
+      <c r="E20" t="n">
+        <v>28.85007950544675</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>COR</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.01431044697378068</v>
+      </c>
+      <c r="C21" t="n">
+        <v>360.239990234375</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1726.459057974628</v>
+      </c>
+      <c r="E21" t="n">
+        <v>4.792524719011291</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>MCK</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.01426431698389305</v>
+      </c>
+      <c r="C22" t="n">
+        <v>858.6099853515625</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1720.893785343263</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2.004278793285445</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>ANET</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.01407159559638884</v>
+      </c>
+      <c r="C23" t="n">
+        <v>134.0200042724609</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1697.643247765249</v>
+      </c>
+      <c r="E23" t="n">
+        <v>12.66708844684083</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>CTSH</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.0137593338650512</v>
+      </c>
+      <c r="C24" t="n">
+        <v>72.83000183105469</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1659.970972712314</v>
+      </c>
+      <c r="E24" t="n">
+        <v>22.79240602743611</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>DLR</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.01310862026768213</v>
+      </c>
+      <c r="C25" t="n">
+        <v>168.3500061035156</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1581.466759225242</v>
+      </c>
+      <c r="E25" t="n">
+        <v>9.393921603144014</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>RTX</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.01310399971079962</v>
+      </c>
+      <c r="C26" t="n">
+        <v>175.1000061035156</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1580.909320153121</v>
+      </c>
+      <c r="E26" t="n">
+        <v>9.028608024253975</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>BMY</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.01309010563502742</v>
+      </c>
+      <c r="C27" t="n">
+        <v>46.63000106811523</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1579.23309347669</v>
+      </c>
+      <c r="E27" t="n">
+        <v>33.86731840665862</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>HSIC</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.01302269742393049</v>
+      </c>
+      <c r="C28" t="n">
+        <v>70.05999755859375</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1571.100746748221</v>
+      </c>
+      <c r="E28" t="n">
+        <v>22.42507567080989</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.01199770199447174</v>
+      </c>
+      <c r="C29" t="n">
+        <v>93.59999847412109</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1447.441950708244</v>
+      </c>
+      <c r="E29" t="n">
+        <v>15.46412365710068</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>WDC</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.0119095215105411</v>
+      </c>
+      <c r="C30" t="n">
+        <v>163.6000061035156</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1436.803569147027</v>
+      </c>
+      <c r="E30" t="n">
+        <v>8.782417576671175</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>KLAC</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0.01153169167723523</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1206.400024414062</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1391.220944140338</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1.153200361394257</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>AES</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0.0110542293712846</v>
+      </c>
+      <c r="C32" t="n">
+        <v>14.1899995803833</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1333.618332254054</v>
+      </c>
+      <c r="E32" t="n">
+        <v>93.9829719302945</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>ED</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.01058413141179475</v>
+      </c>
+      <c r="C33" t="n">
+        <v>96.98999786376953</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1276.904179175283</v>
+      </c>
+      <c r="E33" t="n">
+        <v>13.16531814928793</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>GEHC</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.008557405959917865</v>
+      </c>
+      <c r="C34" t="n">
+        <v>74.16999816894531</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1032.393401780875</v>
+      </c>
+      <c r="E34" t="n">
+        <v>13.919285793014</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>WFC</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.008397108705004578</v>
+      </c>
+      <c r="C35" t="n">
+        <v>85.59000396728516</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1013.054617449361</v>
+      </c>
+      <c r="E35" t="n">
+        <v>11.83613238102639</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>KR</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0.008360355644881825</v>
+      </c>
+      <c r="C36" t="n">
+        <v>63.43000030517578</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1008.620608248008</v>
+      </c>
+      <c r="E36" t="n">
+        <v>15.90131804186207</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>TMO</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0.007981764578775573</v>
+      </c>
+      <c r="C37" t="n">
+        <v>565.97998046875</v>
+      </c>
+      <c r="D37" t="n">
+        <v>962.9461456302465</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1.701378456589092</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>CBRE</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0.007619803472343422</v>
+      </c>
+      <c r="C38" t="n">
+        <v>149.9900054931641</v>
+      </c>
+      <c r="D38" t="n">
+        <v>919.2779756576904</v>
+      </c>
+      <c r="E38" t="n">
+        <v>6.128928208483781</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>AXP</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0.007260345205738991</v>
+      </c>
+      <c r="C39" t="n">
+        <v>365.7300109863281</v>
+      </c>
+      <c r="D39" t="n">
+        <v>875.9117564557247</v>
+      </c>
+      <c r="E39" t="n">
+        <v>2.394968228320941</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>DVA</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0.006670974553374436</v>
+      </c>
+      <c r="C40" t="n">
+        <v>121.5299987792969</v>
+      </c>
+      <c r="D40" t="n">
+        <v>804.8081561877883</v>
+      </c>
+      <c r="E40" t="n">
+        <v>6.622300372514203</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>AXON</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0.006562314583510837</v>
+      </c>
+      <c r="C41" t="n">
+        <v>587.1400146484375</v>
+      </c>
+      <c r="D41" t="n">
+        <v>791.6990625617142</v>
+      </c>
+      <c r="E41" t="n">
+        <v>1.348399091885708</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>HWM</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0.006374120170996832</v>
+      </c>
+      <c r="C42" t="n">
+        <v>205.6000061035156</v>
+      </c>
+      <c r="D42" t="n">
+        <v>768.9946740307122</v>
+      </c>
+      <c r="E42" t="n">
+        <v>3.740246357986674</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>DXCM</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0.006324318836795549</v>
+      </c>
+      <c r="C43" t="n">
+        <v>58.02000045776367</v>
+      </c>
+      <c r="D43" t="n">
+        <v>762.9864784314723</v>
+      </c>
+      <c r="E43" t="n">
+        <v>13.15040455725086</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>UNP</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0.006132148954450109</v>
+      </c>
+      <c r="C44" t="n">
+        <v>217.9900054931641</v>
+      </c>
+      <c r="D44" t="n">
+        <v>739.8024762369165</v>
+      </c>
+      <c r="E44" t="n">
+        <v>3.393744931393728</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>SWK</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0.006109981707425258</v>
+      </c>
+      <c r="C45" t="n">
+        <v>67.47000122070312</v>
+      </c>
+      <c r="D45" t="n">
+        <v>737.1281471620432</v>
+      </c>
+      <c r="E45" t="n">
+        <v>10.92527247407039</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0.005477678446207911</v>
+      </c>
+      <c r="C46" t="n">
+        <v>284.75</v>
+      </c>
+      <c r="D46" t="n">
+        <v>660.8450167527919</v>
+      </c>
+      <c r="E46" t="n">
+        <v>2.320790225646328</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>AVGO</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0.005411273058061387</v>
+      </c>
+      <c r="C47" t="n">
+        <v>355.5899963378906</v>
+      </c>
+      <c r="D47" t="n">
+        <v>652.8336538600787</v>
+      </c>
+      <c r="E47" t="n">
+        <v>1.835916815949287</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>CNC</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0.005222425044578849</v>
+      </c>
+      <c r="C48" t="n">
+        <v>37.09999847412109</v>
+      </c>
+      <c r="D48" t="n">
+        <v>630.050412773703</v>
+      </c>
+      <c r="E48" t="n">
+        <v>16.98249160881209</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0.004828013223446304</v>
+      </c>
+      <c r="C49" t="n">
+        <v>269.7699890136719</v>
+      </c>
+      <c r="D49" t="n">
+        <v>582.4672826021472</v>
+      </c>
+      <c r="E49" t="n">
+        <v>2.159125574834152</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>0.004666330507795211</v>
+      </c>
+      <c r="C50" t="n">
+        <v>475.3800048828125</v>
+      </c>
+      <c r="D50" t="n">
+        <v>562.9613517625866</v>
+      </c>
+      <c r="E50" t="n">
+        <v>1.184234393496134</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>CTRA</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>0.004636741454939017</v>
+      </c>
+      <c r="C51" t="n">
+        <v>26.3700008392334</v>
+      </c>
+      <c r="D51" t="n">
+        <v>559.3916317940865</v>
+      </c>
+      <c r="E51" t="n">
+        <v>21.21318217638512</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>BK</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>0.004617317128190202</v>
+      </c>
+      <c r="C52" t="n">
+        <v>108.4199981689453</v>
+      </c>
+      <c r="D52" t="n">
+        <v>557.0482175791432</v>
+      </c>
+      <c r="E52" t="n">
+        <v>5.13787333505691</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>WST</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>0.004599557749323312</v>
+      </c>
+      <c r="C53" t="n">
+        <v>275.3399963378906</v>
+      </c>
+      <c r="D53" t="n">
+        <v>554.905668114062</v>
+      </c>
+      <c r="E53" t="n">
+        <v>2.015347118088485</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>HCA</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>0.004542133349911796</v>
+      </c>
+      <c r="C54" t="n">
+        <v>471.3599853515625</v>
+      </c>
+      <c r="D54" t="n">
+        <v>547.9778010324532</v>
+      </c>
+      <c r="E54" t="n">
+        <v>1.162546287470171</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>EBAY</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0.004536014304875768</v>
+      </c>
+      <c r="C55" t="n">
+        <v>80.84999847412109</v>
+      </c>
+      <c r="D55" t="n">
+        <v>547.2395794557294</v>
+      </c>
+      <c r="E55" t="n">
+        <v>6.768578723361298</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>0.004009099855122677</v>
+      </c>
+      <c r="C56" t="n">
+        <v>295.2200012207031</v>
+      </c>
+      <c r="D56" t="n">
+        <v>483.6708994403066</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1.638340550912469</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>LKQ</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>0.003996152513895684</v>
+      </c>
+      <c r="C57" t="n">
+        <v>30.02000045776367</v>
+      </c>
+      <c r="D57" t="n">
+        <v>482.1088899112552</v>
+      </c>
+      <c r="E57" t="n">
+        <v>16.05958969219715</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>MMM</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>0.003744251009570338</v>
+      </c>
+      <c r="C58" t="n">
+        <v>163.8500061035156</v>
+      </c>
+      <c r="D58" t="n">
+        <v>451.7186697695126</v>
+      </c>
+      <c r="E58" t="n">
+        <v>2.756903588298495</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>TDY</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>0.003708774963529094</v>
+      </c>
+      <c r="C59" t="n">
+        <v>506.6799926757812</v>
+      </c>
+      <c r="D59" t="n">
+        <v>447.4387237174258</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.8830795180099735</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>VLO</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>0.003273802945045344</v>
+      </c>
+      <c r="C60" t="n">
+        <v>176.0099945068359</v>
+      </c>
+      <c r="D60" t="n">
+        <v>394.9622788759282</v>
+      </c>
+      <c r="E60" t="n">
+        <v>2.24397642862598</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>UAL</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>0.003182191444030683</v>
+      </c>
+      <c r="C61" t="n">
+        <v>95.72000122070312</v>
+      </c>
+      <c r="D61" t="n">
+        <v>383.9099682086795</v>
+      </c>
+      <c r="E61" t="n">
+        <v>4.010760168331927</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>MTD</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>0.003089216179219811</v>
+      </c>
+      <c r="C62" t="n">
+        <v>1439.619995117188</v>
+      </c>
+      <c r="D62" t="n">
+        <v>372.693128623276</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.2588829898774351</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>DAL</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>0.003058950283708984</v>
+      </c>
+      <c r="C63" t="n">
+        <v>57.81000137329102</v>
+      </c>
+      <c r="D63" t="n">
+        <v>369.0417521464884</v>
+      </c>
+      <c r="E63" t="n">
+        <v>6.383700802280045</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>AVB</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>0.003058708953217904</v>
+      </c>
+      <c r="C64" t="n">
+        <v>175.2400054931641</v>
+      </c>
+      <c r="D64" t="n">
+        <v>369.0126372479073</v>
+      </c>
+      <c r="E64" t="n">
+        <v>2.105755681811492</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>WBD</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>0.003018121629956755</v>
+      </c>
+      <c r="C65" t="n">
+        <v>22.42000007629395</v>
+      </c>
+      <c r="D65" t="n">
+        <v>364.116050019602</v>
+      </c>
+      <c r="E65" t="n">
+        <v>16.24068014186157</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>LLY</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0.002406987417346244</v>
+      </c>
+      <c r="C66" t="n">
+        <v>937.4400024414062</v>
+      </c>
+      <c r="D66" t="n">
+        <v>290.3868227681584</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.3097657684885372</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0.002287662708046509</v>
+      </c>
+      <c r="C67" t="n">
+        <v>285.3399963378906</v>
+      </c>
+      <c r="D67" t="n">
+        <v>275.9911001476028</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.9672359419980606</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>DHR</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>0.001948240983821493</v>
+      </c>
+      <c r="C68" t="n">
+        <v>210.6699981689453</v>
+      </c>
+      <c r="D68" t="n">
+        <v>235.0421548536298</v>
+      </c>
+      <c r="E68" t="n">
+        <v>1.115688787660877</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>PLD</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>0.001639085976657081</v>
+      </c>
+      <c r="C69" t="n">
+        <v>124</v>
+      </c>
+      <c r="D69" t="n">
+        <v>197.7446851508928</v>
+      </c>
+      <c r="E69" t="n">
+        <v>1.594715202829781</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>APA</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>0.00150605008169869</v>
+      </c>
+      <c r="C70" t="n">
+        <v>23.63999938964844</v>
+      </c>
+      <c r="D70" t="n">
+        <v>181.6948003144867</v>
+      </c>
+      <c r="E70" t="n">
+        <v>7.685905457089304</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>APD</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>0.001378096196451538</v>
+      </c>
+      <c r="C71" t="n">
+        <v>258.7900085449219</v>
+      </c>
+      <c r="D71" t="n">
+        <v>166.2580257264719</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.642443758401948</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>PSKY</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>0.001228229191631706</v>
+      </c>
+      <c r="C72" t="n">
+        <v>14.80000019073486</v>
+      </c>
+      <c r="D72" t="n">
+        <v>148.1775808293431</v>
+      </c>
+      <c r="E72" t="n">
+        <v>10.0119985756558</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>GILD</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>0.00121430744204888</v>
+      </c>
+      <c r="C73" t="n">
+        <v>123.4000015258789</v>
+      </c>
+      <c r="D73" t="n">
+        <v>146.4980154940211</v>
+      </c>
+      <c r="E73" t="n">
+        <v>1.18718001363475</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>0.001012962749056649</v>
+      </c>
+      <c r="C74" t="n">
+        <v>163.4199981689453</v>
+      </c>
+      <c r="D74" t="n">
+        <v>122.2071341799401</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.7478101551170073</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>TRMB</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>0.0009909054374054613</v>
+      </c>
+      <c r="C75" t="n">
+        <v>78.81999969482422</v>
+      </c>
+      <c r="D75" t="n">
+        <v>119.5460680675723</v>
+      </c>
+      <c r="E75" t="n">
+        <v>1.516697139437092</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>JKHY</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>0.0009101940143863123</v>
+      </c>
+      <c r="C76" t="n">
+        <v>163.0800018310547</v>
+      </c>
+      <c r="D76" t="n">
+        <v>109.8087784071769</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.6733430045023855</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>0.000830419451282133</v>
+      </c>
+      <c r="C77" t="n">
+        <v>170.1000061035156</v>
+      </c>
+      <c r="D77" t="n">
+        <v>100.1845145865205</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.5889741974821122</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>ROL</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>0.0007492526422755881</v>
+      </c>
+      <c r="C78" t="n">
+        <v>58.65000152587891</v>
+      </c>
+      <c r="D78" t="n">
+        <v>90.39228567340609</v>
+      </c>
+      <c r="E78" t="n">
+        <v>1.541215401904485</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>0.0006800956462985395</v>
+      </c>
+      <c r="C79" t="n">
+        <v>445.9100036621094</v>
+      </c>
+      <c r="D79" t="n">
+        <v>82.04895982581748</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.1840034068578343</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>SYK</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>0.0006013042667715897</v>
+      </c>
+      <c r="C80" t="n">
+        <v>353.8099975585938</v>
+      </c>
+      <c r="D80" t="n">
+        <v>72.543310482799</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.2050346541459311</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>FDX</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>0.000596404968009304</v>
+      </c>
+      <c r="C81" t="n">
+        <v>258.8599853515625</v>
+      </c>
+      <c r="D81" t="n">
+        <v>71.95224307998696</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.2779581517099574</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>IBKR</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>0.0005780429331686965</v>
+      </c>
+      <c r="C82" t="n">
+        <v>69.86000061035156</v>
+      </c>
+      <c r="D82" t="n">
+        <v>69.73698723008268</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.9982391443001124</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>XYZ</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>0.0001874957331702002</v>
+      </c>
+      <c r="C83" t="n">
+        <v>70.93000030517578</v>
+      </c>
+      <c r="D83" t="n">
+        <v>22.62009757321833</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0.3189073378809466</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>BR</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>0.0001859591957377702</v>
+      </c>
+      <c r="C84" t="n">
+        <v>217.4900054931641</v>
+      </c>
+      <c r="D84" t="n">
+        <v>22.43472467934603</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0.1031528995020931</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>AVY</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>6.275084676266554e-05</v>
+      </c>
+      <c r="C85" t="n">
+        <v>171.9499969482422</v>
+      </c>
+      <c r="D85" t="n">
+        <v>7.570467085163328</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0.04402714288760398</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G85"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Shares</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Entry_Price</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Exit_Price</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Sale_Value</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Transaction_Cost</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Gain_Loss</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>LRCX</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>59.00353783170021</v>
+      </c>
+      <c r="C2" t="n">
+        <v>162.1900024414062</v>
+      </c>
+      <c r="D2" t="n">
+        <v>159.3500061035156</v>
+      </c>
+      <c r="E2" t="n">
+        <v>9402.214113610444</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-167.5698313646189</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>AMAT</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>39.28056215278161</v>
+      </c>
+      <c r="C3" t="n">
+        <v>233.5299987792969</v>
+      </c>
+      <c r="D3" t="n">
+        <v>230.0700073242188</v>
+      </c>
+      <c r="E3" t="n">
+        <v>9037.279222189896</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-135.9104093992883</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>BIIB</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>44.46901056755588</v>
+      </c>
+      <c r="C4" t="n">
+        <v>156.7400054931641</v>
+      </c>
+      <c r="D4" t="n">
+        <v>155.5099945068359</v>
+      </c>
+      <c r="E4" t="n">
+        <v>6915.375589085043</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-54.69737154923587</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>HOOD</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>50.95672031917098</v>
+      </c>
+      <c r="C5" t="n">
+        <v>127.0800018310547</v>
+      </c>
+      <c r="D5" t="n">
+        <v>130.3600006103516</v>
+      </c>
+      <c r="E5" t="n">
+        <v>6642.718091908642</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>167.1379804438529</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>TEL</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>20.52036958935327</v>
+      </c>
+      <c r="C6" t="n">
+        <v>242.5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>242.4199981689453</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4974.547958277101</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-1.641667141067046</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>20.32369270285715</v>
+      </c>
+      <c r="C7" t="n">
+        <v>243.0399932861328</v>
+      </c>
+      <c r="D7" t="n">
+        <v>244.4100036621094</v>
+      </c>
+      <c r="E7" t="n">
+        <v>4967.313807932902</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>27.84366988107377</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>CSCO</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>63.95395729108021</v>
+      </c>
+      <c r="C8" t="n">
+        <v>71.04000091552734</v>
+      </c>
+      <c r="D8" t="n">
+        <v>71.06999969482422</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4545.207725159871</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.918540649936403</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>CEG</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>9.746663887646196</v>
+      </c>
+      <c r="C9" t="n">
+        <v>351.2999877929688</v>
+      </c>
+      <c r="D9" t="n">
+        <v>358.3900146484375</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3493.107013466917</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>69.1041087146391</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ISRG</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>5.841020406573547</v>
+      </c>
+      <c r="C10" t="n">
+        <v>547.780029296875</v>
+      </c>
+      <c r="D10" t="n">
+        <v>560</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3270.971427681186</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>71.37709824468402</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>EXE</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>28.61410253876072</v>
+      </c>
+      <c r="C11" t="n">
+        <v>110.620002746582</v>
+      </c>
+      <c r="D11" t="n">
+        <v>112.4499969482422</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3217.655743160331</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>52.36364173164111</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>EL</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>36.01079205759416</v>
+      </c>
+      <c r="C12" t="n">
+        <v>87.77999877929688</v>
+      </c>
+      <c r="D12" t="n">
+        <v>87.75</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3159.947003053887</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-1.08027980324141</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>7.83506761144009</v>
+      </c>
+      <c r="C13" t="n">
+        <v>371.1600036621094</v>
+      </c>
+      <c r="D13" t="n">
+        <v>371.6900024414062</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2912.21629962475</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>4.152576269771998</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>41.11974059577549</v>
+      </c>
+      <c r="C14" t="n">
+        <v>68.83999633789062</v>
+      </c>
+      <c r="D14" t="n">
+        <v>70.75</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2909.221647151116</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>78.5388551229189</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>GL</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>20.46026733652463</v>
+      </c>
+      <c r="C15" t="n">
+        <v>131.8300018310547</v>
+      </c>
+      <c r="D15" t="n">
+        <v>132.2400054931641</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2705.665864973622</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>8.388784535711693</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>FSLR</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>7.589351457187063</v>
+      </c>
+      <c r="C16" t="n">
+        <v>271.9800109863281</v>
+      </c>
+      <c r="D16" t="n">
+        <v>267.6400146484375</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2031.214135173686</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>-32.93775753115665</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>DLTR</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>19.46491085553966</v>
+      </c>
+      <c r="C17" t="n">
+        <v>101.9700012207031</v>
+      </c>
+      <c r="D17" t="n">
+        <v>105.7399978637695</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2058.219632283228</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>73.38264858297134</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>GLW</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>22.52897530009663</v>
+      </c>
+      <c r="C18" t="n">
+        <v>87.86000061035156</v>
+      </c>
+      <c r="D18" t="n">
+        <v>85.48000335693359</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1925.776884280534</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>-53.61889933655107</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>CVS</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>24.24883805820526</v>
+      </c>
+      <c r="C19" t="n">
+        <v>78.66000366210938</v>
+      </c>
+      <c r="D19" t="n">
+        <v>78.98999786376953</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1915.415666416527</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>8.001975956203751</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>28.85007950544675</v>
+      </c>
+      <c r="C20" t="n">
+        <v>60.5</v>
+      </c>
+      <c r="D20" t="n">
+        <v>61.58000183105469</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1776.587948771484</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>31.15813869195586</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>COR</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>4.792524719011291</v>
+      </c>
+      <c r="C21" t="n">
+        <v>360.239990234375</v>
+      </c>
+      <c r="D21" t="n">
+        <v>360.7000122070312</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1728.663724649871</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>2.204666675243288</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>MCK</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>2.004278793285445</v>
+      </c>
+      <c r="C22" t="n">
+        <v>858.6099853515625</v>
+      </c>
+      <c r="D22" t="n">
+        <v>851.989990234375</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1707.625469518231</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>-13.268315825032</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>ANET</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>12.66708844684083</v>
+      </c>
+      <c r="C23" t="n">
+        <v>134.0200042724609</v>
+      </c>
+      <c r="D23" t="n">
+        <v>134.6499938964844</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1705.623382053345</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>7.980134288096906</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>CTSH</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>22.79240602743611</v>
+      </c>
+      <c r="C24" t="n">
+        <v>72.83000183105469</v>
+      </c>
+      <c r="D24" t="n">
+        <v>73.19999694824219</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1668.40405165142</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>8.433078939106281</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>DLR</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>9.393921603144014</v>
+      </c>
+      <c r="C25" t="n">
+        <v>168.3500061035156</v>
+      </c>
+      <c r="D25" t="n">
+        <v>169.8899993896484</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1595.933335424542</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>14.46657619929988</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>RTX</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>9.028608024253975</v>
+      </c>
+      <c r="C26" t="n">
+        <v>175.1000061035156</v>
+      </c>
+      <c r="D26" t="n">
+        <v>176.9700012207031</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1597.792773073476</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>16.88345292035478</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>BMY</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>33.86731840665862</v>
+      </c>
+      <c r="C27" t="n">
+        <v>46.63000106811523</v>
+      </c>
+      <c r="D27" t="n">
+        <v>46.68999862670898</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1581.265049897207</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>2.031956420516735</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>HSIC</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>22.42507567080989</v>
+      </c>
+      <c r="C28" t="n">
+        <v>70.05999755859375</v>
+      </c>
+      <c r="D28" t="n">
+        <v>71.90000152587891</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1612.362974949181</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>41.26222820095995</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>15.46412365710068</v>
+      </c>
+      <c r="C29" t="n">
+        <v>93.59999847412109</v>
+      </c>
+      <c r="D29" t="n">
+        <v>95.94999694824219</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1483.78261770605</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>36.34066699780647</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>WDC</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>8.782417576671175</v>
+      </c>
+      <c r="C30" t="n">
+        <v>163.6000061035156</v>
+      </c>
+      <c r="D30" t="n">
+        <v>162.9600067138672</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1431.18282725832</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>-5.620741888707244</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>KLAC</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1.153200361394257</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1206.400024414062</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1193.369995117188</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1376.194709646204</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>-15.02623449413409</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>AES</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>93.9829719302945</v>
+      </c>
+      <c r="C32" t="n">
+        <v>14.1899995803833</v>
+      </c>
+      <c r="D32" t="n">
+        <v>14.13000011444092</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1327.979404130559</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>-5.638928123495589</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>ED</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>13.16531814928793</v>
+      </c>
+      <c r="C33" t="n">
+        <v>96.98999786376953</v>
+      </c>
+      <c r="D33" t="n">
+        <v>98.51999664306641</v>
+      </c>
+      <c r="E33" t="n">
+        <v>1297.047099872748</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>20.14292069746534</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>GEHC</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>13.919285793014</v>
+      </c>
+      <c r="C34" t="n">
+        <v>74.16999816894531</v>
+      </c>
+      <c r="D34" t="n">
+        <v>73.05000305175781</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1016.803869657962</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>-15.58953212291306</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>WFC</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>11.83613238102639</v>
+      </c>
+      <c r="C35" t="n">
+        <v>85.59000396728516</v>
+      </c>
+      <c r="D35" t="n">
+        <v>86.04000091552734</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1018.380840899813</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>5.326223450452403</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>KR</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>15.90131804186207</v>
+      </c>
+      <c r="C36" t="n">
+        <v>63.43000030517578</v>
+      </c>
+      <c r="D36" t="n">
+        <v>64.91000366210938</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1032.154612329633</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>23.53400408162463</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>TMO</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>1.701378456589092</v>
+      </c>
+      <c r="C37" t="n">
+        <v>565.97998046875</v>
+      </c>
+      <c r="D37" t="n">
+        <v>572.4099731445312</v>
+      </c>
+      <c r="E37" t="n">
+        <v>973.8859966448464</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>10.93985101459987</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>CBRE</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>6.128928208483781</v>
+      </c>
+      <c r="C38" t="n">
+        <v>149.9900054931641</v>
+      </c>
+      <c r="D38" t="n">
+        <v>152.6499938964844</v>
+      </c>
+      <c r="E38" t="n">
+        <v>935.58085361704</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>16.30287795934964</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>AXP</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>2.394968228320941</v>
+      </c>
+      <c r="C39" t="n">
+        <v>365.7300109863281</v>
+      </c>
+      <c r="D39" t="n">
+        <v>368.5400085449219</v>
+      </c>
+      <c r="E39" t="n">
+        <v>882.6416113302161</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>6.729854874491366</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>DVA</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>6.622300372514203</v>
+      </c>
+      <c r="C40" t="n">
+        <v>121.5299987792969</v>
+      </c>
+      <c r="D40" t="n">
+        <v>123.6900024414062</v>
+      </c>
+      <c r="E40" t="n">
+        <v>819.1123492440072</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>14.30419305621888</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>AXON</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>1.348399091885708</v>
+      </c>
+      <c r="C41" t="n">
+        <v>587.1400146484375</v>
+      </c>
+      <c r="D41" t="n">
+        <v>602.510009765625</v>
+      </c>
+      <c r="E41" t="n">
+        <v>812.4239500200176</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>20.72488745830344</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>HWM</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>3.740246357986674</v>
+      </c>
+      <c r="C42" t="n">
+        <v>205.6000061035156</v>
+      </c>
+      <c r="D42" t="n">
+        <v>206.6600036621094</v>
+      </c>
+      <c r="E42" t="n">
+        <v>772.9593260387172</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>3.964652008005032</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>DXCM</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>13.15040455725086</v>
+      </c>
+      <c r="C43" t="n">
+        <v>58.02000045776367</v>
+      </c>
+      <c r="D43" t="n">
+        <v>55</v>
+      </c>
+      <c r="E43" t="n">
+        <v>723.2722506487972</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>-39.71422778267504</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>UNP</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>3.393744931393728</v>
+      </c>
+      <c r="C44" t="n">
+        <v>217.9900054931641</v>
+      </c>
+      <c r="D44" t="n">
+        <v>221.4799957275391</v>
+      </c>
+      <c r="E44" t="n">
+        <v>751.6466129054403</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>11.84413666852379</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>SWK</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>10.92527247407039</v>
+      </c>
+      <c r="C45" t="n">
+        <v>67.47000122070312</v>
+      </c>
+      <c r="D45" t="n">
+        <v>68.26999664306641</v>
+      </c>
+      <c r="E45" t="n">
+        <v>745.8683151293711</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>8.74016796732792</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>2.320790225646328</v>
+      </c>
+      <c r="C46" t="n">
+        <v>284.75</v>
+      </c>
+      <c r="D46" t="n">
+        <v>278.8299865722656</v>
+      </c>
+      <c r="E46" t="n">
+        <v>647.1059074540109</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>-13.73910929878105</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>AVGO</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>1.835916815949287</v>
+      </c>
+      <c r="C47" t="n">
+        <v>355.5899963378906</v>
+      </c>
+      <c r="D47" t="n">
+        <v>349.4299926757812</v>
+      </c>
+      <c r="E47" t="n">
+        <v>641.5243995505028</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>-11.30925430957586</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>CNC</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>16.98249160881209</v>
+      </c>
+      <c r="C48" t="n">
+        <v>37.09999847412109</v>
+      </c>
+      <c r="D48" t="n">
+        <v>37.56000137329102</v>
+      </c>
+      <c r="E48" t="n">
+        <v>637.8624081488854</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>7.811995375182391</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>2.159125574834152</v>
+      </c>
+      <c r="C49" t="n">
+        <v>269.7699890136719</v>
+      </c>
+      <c r="D49" t="n">
+        <v>268.4700012207031</v>
+      </c>
+      <c r="E49" t="n">
+        <v>579.6604457113762</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>-2.806836890771024</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>1.184234393496134</v>
+      </c>
+      <c r="C50" t="n">
+        <v>475.3800048828125</v>
+      </c>
+      <c r="D50" t="n">
+        <v>467.7900085449219</v>
+      </c>
+      <c r="E50" t="n">
+        <v>553.9730170527467</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>-8.988334709839819</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>CTRA</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>21.21318217638512</v>
+      </c>
+      <c r="C51" t="n">
+        <v>26.3700008392334</v>
+      </c>
+      <c r="D51" t="n">
+        <v>26.56999969482422</v>
+      </c>
+      <c r="E51" t="n">
+        <v>563.6342439528031</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>4.242612158716611</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>BK</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>5.13787333505691</v>
+      </c>
+      <c r="C52" t="n">
+        <v>108.4199981689453</v>
+      </c>
+      <c r="D52" t="n">
+        <v>109.6399993896484</v>
+      </c>
+      <c r="E52" t="n">
+        <v>563.3164293197306</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="n">
+        <v>6.26821174058739</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>WST</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>2.015347118088485</v>
+      </c>
+      <c r="C53" t="n">
+        <v>275.3399963378906</v>
+      </c>
+      <c r="D53" t="n">
+        <v>271.0400085449219</v>
+      </c>
+      <c r="E53" t="n">
+        <v>546.2397001076868</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" t="n">
+        <v>-8.665968006375238</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>HCA</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>1.162546287470171</v>
+      </c>
+      <c r="C54" t="n">
+        <v>471.3599853515625</v>
+      </c>
+      <c r="D54" t="n">
+        <v>476.6099853515625</v>
+      </c>
+      <c r="E54" t="n">
+        <v>554.0811690416716</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="n">
+        <v>6.103368009218457</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>EBAY</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>6.768578723361298</v>
+      </c>
+      <c r="C55" t="n">
+        <v>80.84999847412109</v>
+      </c>
+      <c r="D55" t="n">
+        <v>83.80000305175781</v>
+      </c>
+      <c r="E55" t="n">
+        <v>567.2069176737398</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" t="n">
+        <v>19.96733821801035</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>COIN</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>1.638340550912469</v>
+      </c>
+      <c r="C56" t="n">
+        <v>295.2200012207031</v>
+      </c>
+      <c r="D56" t="n">
+        <v>309.1400146484375</v>
+      </c>
+      <c r="E56" t="n">
+        <v>506.4766219082098</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" t="n">
+        <v>22.80572246790325</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>LKQ</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>16.05958969219715</v>
+      </c>
+      <c r="C57" t="n">
+        <v>30.02000045776367</v>
+      </c>
+      <c r="D57" t="n">
+        <v>30.3700008392334</v>
+      </c>
+      <c r="E57" t="n">
+        <v>487.7297524297715</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" t="n">
+        <v>5.620862518516333</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>MMM</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>2.756903588298495</v>
+      </c>
+      <c r="C58" t="n">
+        <v>163.8500061035156</v>
+      </c>
+      <c r="D58" t="n">
+        <v>164.8399963378906</v>
+      </c>
+      <c r="E58" t="n">
+        <v>454.4479773990415</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" t="n">
+        <v>2.729307629528932</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>TDY</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>0.8830795180099735</v>
+      </c>
+      <c r="C59" t="n">
+        <v>506.6799926757812</v>
+      </c>
+      <c r="D59" t="n">
+        <v>513.1699829101562</v>
+      </c>
+      <c r="E59" t="n">
+        <v>453.1699011654871</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" t="n">
+        <v>5.731177448061317</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>VLO</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>2.24397642862598</v>
+      </c>
+      <c r="C60" t="n">
+        <v>176.0099945068359</v>
+      </c>
+      <c r="D60" t="n">
+        <v>175.6199951171875</v>
+      </c>
+      <c r="E60" t="n">
+        <v>394.0871294383786</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" t="n">
+        <v>-0.8751494375495668</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>UAL</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>4.010760168331927</v>
+      </c>
+      <c r="C61" t="n">
+        <v>95.72000122070312</v>
+      </c>
+      <c r="D61" t="n">
+        <v>97.43000030517578</v>
+      </c>
+      <c r="E61" t="n">
+        <v>390.7683644245665</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="n">
+        <v>6.858396215887012</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>MTD</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>0.2588829898774351</v>
+      </c>
+      <c r="C62" t="n">
+        <v>1439.619995117188</v>
+      </c>
+      <c r="D62" t="n">
+        <v>1439.349975585938</v>
+      </c>
+      <c r="E62" t="n">
+        <v>372.6232251597008</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" t="n">
+        <v>-0.06990346357525823</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>DAL</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>6.383700802280045</v>
+      </c>
+      <c r="C63" t="n">
+        <v>57.81000137329102</v>
+      </c>
+      <c r="D63" t="n">
+        <v>58.88000106811523</v>
+      </c>
+      <c r="E63" t="n">
+        <v>375.8723100567772</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0</v>
+      </c>
+      <c r="G63" t="n">
+        <v>6.830557910288803</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>AVB</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>2.105755681811492</v>
+      </c>
+      <c r="C64" t="n">
+        <v>175.2400054931641</v>
+      </c>
+      <c r="D64" t="n">
+        <v>177.3800048828125</v>
+      </c>
+      <c r="E64" t="n">
+        <v>373.5189531217326</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G64" t="n">
+        <v>4.506315873825372</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>WBD</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>16.24068014186157</v>
+      </c>
+      <c r="C65" t="n">
+        <v>22.42000007629395</v>
+      </c>
+      <c r="D65" t="n">
+        <v>22.67000007629395</v>
+      </c>
+      <c r="E65" t="n">
+        <v>368.1762200550675</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0</v>
+      </c>
+      <c r="G65" t="n">
+        <v>4.060170035465376</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>LLY</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0.3097657684885372</v>
+      </c>
+      <c r="C66" t="n">
+        <v>937.4400024414062</v>
+      </c>
+      <c r="D66" t="n">
+        <v>924.3699951171875</v>
+      </c>
+      <c r="E66" t="n">
+        <v>286.3381819052209</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" t="n">
+        <v>-4.048640862937475</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0.9672359419980606</v>
+      </c>
+      <c r="C67" t="n">
+        <v>285.3399963378906</v>
+      </c>
+      <c r="D67" t="n">
+        <v>279.7000122070312</v>
+      </c>
+      <c r="E67" t="n">
+        <v>270.5359047839369</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0</v>
+      </c>
+      <c r="G67" t="n">
+        <v>-5.455195363665894</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>DHR</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>1.115688787660877</v>
+      </c>
+      <c r="C68" t="n">
+        <v>210.6699981689453</v>
+      </c>
+      <c r="D68" t="n">
+        <v>209.9400024414062</v>
+      </c>
+      <c r="E68" t="n">
+        <v>234.2277068053741</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" t="n">
+        <v>-0.8144480482556844</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>PLD</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>1.594715202829781</v>
+      </c>
+      <c r="C69" t="n">
+        <v>124</v>
+      </c>
+      <c r="D69" t="n">
+        <v>125.5999984741211</v>
+      </c>
+      <c r="E69" t="n">
+        <v>200.2962270420782</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0</v>
+      </c>
+      <c r="G69" t="n">
+        <v>2.551541891185366</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>APA</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>7.685905457089304</v>
+      </c>
+      <c r="C70" t="n">
+        <v>23.63999938964844</v>
+      </c>
+      <c r="D70" t="n">
+        <v>23.82999992370605</v>
+      </c>
+      <c r="E70" t="n">
+        <v>183.1551264560501</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" t="n">
+        <v>1.460326141563314</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>APD</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>0.642443758401948</v>
+      </c>
+      <c r="C71" t="n">
+        <v>258.7900085449219</v>
+      </c>
+      <c r="D71" t="n">
+        <v>259.739990234375</v>
+      </c>
+      <c r="E71" t="n">
+        <v>166.8683355334572</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0.610309806985299</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>PSKY</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>10.0119985756558</v>
+      </c>
+      <c r="C72" t="n">
+        <v>14.80000019073486</v>
+      </c>
+      <c r="D72" t="n">
+        <v>15.10000038146973</v>
+      </c>
+      <c r="E72" t="n">
+        <v>151.181182311677</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0</v>
+      </c>
+      <c r="G72" t="n">
+        <v>3.00360148233392</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>GILD</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>1.18718001363475</v>
+      </c>
+      <c r="C73" t="n">
+        <v>123.4000015258789</v>
+      </c>
+      <c r="D73" t="n">
+        <v>118.8399963378906</v>
+      </c>
+      <c r="E73" t="n">
+        <v>141.0844684727706</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0</v>
+      </c>
+      <c r="G73" t="n">
+        <v>-5.413547021250452</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>MS</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>0.7478101551170073</v>
+      </c>
+      <c r="C74" t="n">
+        <v>163.4199981689453</v>
+      </c>
+      <c r="D74" t="n">
+        <v>162.3600006103516</v>
+      </c>
+      <c r="E74" t="n">
+        <v>121.4144572412244</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" t="n">
+        <v>-0.7926769387156298</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>TRMB</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>1.516697139437092</v>
+      </c>
+      <c r="C75" t="n">
+        <v>78.81999969482422</v>
+      </c>
+      <c r="D75" t="n">
+        <v>78.90000152587891</v>
+      </c>
+      <c r="E75" t="n">
+        <v>119.6674066158827</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0.1213385483103764</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>JKHY</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>0.6733430045023855</v>
+      </c>
+      <c r="C76" t="n">
+        <v>163.0800018310547</v>
+      </c>
+      <c r="D76" t="n">
+        <v>160.8000030517578</v>
+      </c>
+      <c r="E76" t="n">
+        <v>108.2735571788634</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G76" t="n">
+        <v>-1.535221228313532</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>0.5889741974821122</v>
+      </c>
+      <c r="C77" t="n">
+        <v>170.1000061035156</v>
+      </c>
+      <c r="D77" t="n">
+        <v>172.5</v>
+      </c>
+      <c r="E77" t="n">
+        <v>101.5980490656644</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0</v>
+      </c>
+      <c r="G77" t="n">
+        <v>1.413534479143848</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>ROL</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>1.541215401904485</v>
+      </c>
+      <c r="C78" t="n">
+        <v>58.65000152587891</v>
+      </c>
+      <c r="D78" t="n">
+        <v>58.61000061035156</v>
+      </c>
+      <c r="E78" t="n">
+        <v>90.33063564630507</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0</v>
+      </c>
+      <c r="G78" t="n">
+        <v>-0.06165002710102385</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>0.1840034068578343</v>
+      </c>
+      <c r="C79" t="n">
+        <v>445.9100036621094</v>
+      </c>
+      <c r="D79" t="n">
+        <v>429.5199890136719</v>
+      </c>
+      <c r="E79" t="n">
+        <v>79.03314129205516</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0</v>
+      </c>
+      <c r="G79" t="n">
+        <v>-3.015818533762314</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>SYK</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>0.2050346541459311</v>
+      </c>
+      <c r="C80" t="n">
+        <v>353.8099975585938</v>
+      </c>
+      <c r="D80" t="n">
+        <v>356.0299987792969</v>
+      </c>
+      <c r="E80" t="n">
+        <v>72.99848766528942</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0.4551771824904165</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>FDX</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>0.2779581517099574</v>
+      </c>
+      <c r="C81" t="n">
+        <v>258.8599853515625</v>
+      </c>
+      <c r="D81" t="n">
+        <v>262.0899963378906</v>
+      </c>
+      <c r="E81" t="n">
+        <v>72.85005096374958</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0</v>
+      </c>
+      <c r="G81" t="n">
+        <v>0.8978078837626242</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>IBKR</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>0.9982391443001124</v>
+      </c>
+      <c r="C82" t="n">
+        <v>69.86000061035156</v>
+      </c>
+      <c r="D82" t="n">
+        <v>70.54000091552734</v>
+      </c>
+      <c r="E82" t="n">
+        <v>70.41579015284516</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0</v>
+      </c>
+      <c r="G82" t="n">
+        <v>0.6788029227624861</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>XYZ</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>0.3189073378809466</v>
+      </c>
+      <c r="C83" t="n">
+        <v>70.93000030517578</v>
+      </c>
+      <c r="D83" t="n">
+        <v>65.44999694824219</v>
+      </c>
+      <c r="E83" t="n">
+        <v>20.87248429107999</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0</v>
+      </c>
+      <c r="G83" t="n">
+        <v>-1.747613282138342</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>BR</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>0.1031528995020931</v>
+      </c>
+      <c r="C84" t="n">
+        <v>217.4900054931641</v>
+      </c>
+      <c r="D84" t="n">
+        <v>221.7200012207031</v>
+      </c>
+      <c r="E84" t="n">
+        <v>22.87106100352315</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" t="n">
+        <v>0.4363363241771196</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>AVY</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>0.04402714288760398</v>
+      </c>
+      <c r="C85" t="n">
+        <v>171.9499969482422</v>
+      </c>
+      <c r="D85" t="n">
+        <v>174.0700073242188</v>
+      </c>
+      <c r="E85" t="n">
+        <v>7.663805084909651</v>
+      </c>
+      <c r="F85" t="n">
+        <v>0</v>
+      </c>
+      <c r="G85" t="n">
+        <v>0.09333799974632306</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
save for now, quantized doesnt work
</commit_message>
<xml_diff>
--- a/backtest_portfolio_PL.xlsx
+++ b/backtest_portfolio_PL.xlsx
@@ -46,6 +46,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="11-17-2025_PnL" sheetId="38" state="visible" r:id="rId38"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="11-18-2025_Allocations" sheetId="39" state="visible" r:id="rId39"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="11-18-2025_PnL" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="11-19-2025_Allocations" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="11-19-2025_PnL" sheetId="42" state="visible" r:id="rId42"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -72809,6 +72811,3584 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E80"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Allocation_Percent</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Entry_Price</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Target_Value</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Actual_Shares</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CAH</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.05595291331439447</v>
+      </c>
+      <c r="C2" t="n">
+        <v>206.9700012207031</v>
+      </c>
+      <c r="D2" t="n">
+        <v>6703.061209371984</v>
+      </c>
+      <c r="E2" t="n">
+        <v>32.38663173328271</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>COR</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.05428906677149338</v>
+      </c>
+      <c r="C3" t="n">
+        <v>361.6400146484375</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6503.73530193619</v>
+      </c>
+      <c r="E3" t="n">
+        <v>17.98400353527994</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>DD</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.04336015848661273</v>
+      </c>
+      <c r="C4" t="n">
+        <v>38.70000076293945</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5194.47119313917</v>
+      </c>
+      <c r="E4" t="n">
+        <v>134.2240591921018</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>WELL</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.03370516643660074</v>
+      </c>
+      <c r="C5" t="n">
+        <v>198.2899932861328</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4037.820022473838</v>
+      </c>
+      <c r="E5" t="n">
+        <v>20.36320620903575</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>INCY</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.02870592674810414</v>
+      </c>
+      <c r="C6" t="n">
+        <v>103.8899993896484</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3438.91984646292</v>
+      </c>
+      <c r="E6" t="n">
+        <v>33.1015484326355</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>VTR</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.02855550059394055</v>
+      </c>
+      <c r="C7" t="n">
+        <v>79.86000061035156</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3420.899056139039</v>
+      </c>
+      <c r="E7" t="n">
+        <v>42.83620122707109</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>AEP</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.027509336904297</v>
+      </c>
+      <c r="C8" t="n">
+        <v>123.5100021362305</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3295.570474813872</v>
+      </c>
+      <c r="E8" t="n">
+        <v>26.68262017499511</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>EXPD</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.02639293119993945</v>
+      </c>
+      <c r="C9" t="n">
+        <v>139.9100036621094</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3161.827022909009</v>
+      </c>
+      <c r="E9" t="n">
+        <v>22.59900607639895</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>MCK</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.02547673805182647</v>
+      </c>
+      <c r="C10" t="n">
+        <v>860.75</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3052.068685270696</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3.54582478683787</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>AKAM</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.02319227442048374</v>
+      </c>
+      <c r="C11" t="n">
+        <v>87.73999786376953</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2778.393935478266</v>
+      </c>
+      <c r="E11" t="n">
+        <v>31.6662184080762</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>HCA</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.02265052426022807</v>
+      </c>
+      <c r="C12" t="n">
+        <v>478.1400146484375</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2713.493213258916</v>
+      </c>
+      <c r="E12" t="n">
+        <v>5.675101706879875</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>LVS</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.02199007093218165</v>
+      </c>
+      <c r="C13" t="n">
+        <v>64.77999877929688</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2634.372059031372</v>
+      </c>
+      <c r="E13" t="n">
+        <v>40.66644193690993</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>LLY</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.02093350977986882</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1030.050048828125</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2507.797879853189</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2.434636921483844</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>WDC</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.01840686499171431</v>
+      </c>
+      <c r="C15" t="n">
+        <v>152.8600006103516</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2205.110250807369</v>
+      </c>
+      <c r="E15" t="n">
+        <v>14.42568521524682</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>AMGN</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.0182613241276406</v>
+      </c>
+      <c r="C16" t="n">
+        <v>343.989990234375</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2187.674709696769</v>
+      </c>
+      <c r="E16" t="n">
+        <v>6.359704560607165</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>CTRA</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.01803647025227119</v>
+      </c>
+      <c r="C17" t="n">
+        <v>26.17000007629395</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2160.737608472087</v>
+      </c>
+      <c r="E17" t="n">
+        <v>82.56544142807964</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>EPAM</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.01675115152189918</v>
+      </c>
+      <c r="C18" t="n">
+        <v>178.7100067138672</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2006.758671310661</v>
+      </c>
+      <c r="E18" t="n">
+        <v>11.22913432891134</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>UHS</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.01663385742464613</v>
+      </c>
+      <c r="C19" t="n">
+        <v>228.8399963378906</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1992.707043489828</v>
+      </c>
+      <c r="E19" t="n">
+        <v>8.707861717265208</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>EW</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.01640224208500541</v>
+      </c>
+      <c r="C20" t="n">
+        <v>84.04000091552734</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1964.959930664483</v>
+      </c>
+      <c r="E20" t="n">
+        <v>23.38124594548207</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.01618045371279322</v>
+      </c>
+      <c r="C21" t="n">
+        <v>284.2799987792969</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1938.390071359538</v>
+      </c>
+      <c r="E21" t="n">
+        <v>6.818594623902554</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>ISRG</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.01611187778398201</v>
+      </c>
+      <c r="C22" t="n">
+        <v>546.77001953125</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1930.174794958678</v>
+      </c>
+      <c r="E22" t="n">
+        <v>3.530140143041185</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>DDOG</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.01596456654056113</v>
+      </c>
+      <c r="C23" t="n">
+        <v>176.4600067138672</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1912.52716549691</v>
+      </c>
+      <c r="E23" t="n">
+        <v>10.8383038236993</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.01565549805255847</v>
+      </c>
+      <c r="C24" t="n">
+        <v>284.9599914550781</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1875.501300885909</v>
+      </c>
+      <c r="E24" t="n">
+        <v>6.581630253809045</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>MU</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.01564482452376371</v>
+      </c>
+      <c r="C25" t="n">
+        <v>228.5</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1874.222630793625</v>
+      </c>
+      <c r="E25" t="n">
+        <v>8.202287224479758</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.01529158721343493</v>
+      </c>
+      <c r="C26" t="n">
+        <v>817.2999877929688</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1831.905418475055</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2.241411288187976</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>CMI</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.01518686318271681</v>
+      </c>
+      <c r="C27" t="n">
+        <v>464.9200134277344</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1819.35966265263</v>
+      </c>
+      <c r="E27" t="n">
+        <v>3.913274563594206</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.0150819823017463</v>
+      </c>
+      <c r="C28" t="n">
+        <v>546.8800048828125</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1806.795116444143</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3.303823691325687</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>PFE</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.0149641641715429</v>
+      </c>
+      <c r="C29" t="n">
+        <v>25.45000076293945</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1792.680710391867</v>
+      </c>
+      <c r="E29" t="n">
+        <v>70.43931853245313</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>EQT</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.01459682656973934</v>
+      </c>
+      <c r="C30" t="n">
+        <v>58.75</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1748.674307801929</v>
+      </c>
+      <c r="E30" t="n">
+        <v>29.764669068969</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>FDS</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0.01406063358063434</v>
+      </c>
+      <c r="C31" t="n">
+        <v>272.1099853515625</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1684.439324972495</v>
+      </c>
+      <c r="E31" t="n">
+        <v>6.190288543789459</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>FDX</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0.01401212328101446</v>
+      </c>
+      <c r="C32" t="n">
+        <v>263.0799865722656</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1678.627875874037</v>
+      </c>
+      <c r="E32" t="n">
+        <v>6.380674933678142</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.01399390589632981</v>
+      </c>
+      <c r="C33" t="n">
+        <v>376.6300048828125</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1676.445465032804</v>
+      </c>
+      <c r="E33" t="n">
+        <v>4.451173415018875</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>ES</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.01398901893831444</v>
+      </c>
+      <c r="C34" t="n">
+        <v>74.54000091552734</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1675.860016004965</v>
+      </c>
+      <c r="E34" t="n">
+        <v>22.48269379422383</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>EXE</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.01392859628559638</v>
+      </c>
+      <c r="C35" t="n">
+        <v>117.1600036621094</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1668.621487828139</v>
+      </c>
+      <c r="E35" t="n">
+        <v>14.24224509791294</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>DHR</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0.01306050092077547</v>
+      </c>
+      <c r="C36" t="n">
+        <v>225.5099945068359</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1564.625180553292</v>
+      </c>
+      <c r="E36" t="n">
+        <v>6.93816335712723</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>JKHY</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0.01234152136314921</v>
+      </c>
+      <c r="C37" t="n">
+        <v>163.9400024414062</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1478.492686325932</v>
+      </c>
+      <c r="E37" t="n">
+        <v>9.018498623326296</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>MAR</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0.01201676187403415</v>
+      </c>
+      <c r="C38" t="n">
+        <v>282.8999938964844</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1439.587067209535</v>
+      </c>
+      <c r="E38" t="n">
+        <v>5.088678325444903</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>TMO</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0.01195812358149612</v>
+      </c>
+      <c r="C39" t="n">
+        <v>576.030029296875</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1432.562302263215</v>
+      </c>
+      <c r="E39" t="n">
+        <v>2.486957674779311</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>EXPE</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0.01146366382394126</v>
+      </c>
+      <c r="C40" t="n">
+        <v>239.6000061035156</v>
+      </c>
+      <c r="D40" t="n">
+        <v>1373.326887623799</v>
+      </c>
+      <c r="E40" t="n">
+        <v>5.731748132888083</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0.01036361996008058</v>
+      </c>
+      <c r="C41" t="n">
+        <v>67.93000030517578</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1241.543555609963</v>
+      </c>
+      <c r="E41" t="n">
+        <v>18.27680774374096</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>BIIB</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0.01005458276199657</v>
+      </c>
+      <c r="C42" t="n">
+        <v>168.8300018310547</v>
+      </c>
+      <c r="D42" t="n">
+        <v>1204.521439476521</v>
+      </c>
+      <c r="E42" t="n">
+        <v>7.134522456985254</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>CHRW</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0.009796152585946358</v>
+      </c>
+      <c r="C43" t="n">
+        <v>151.6900024414062</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1173.561956121653</v>
+      </c>
+      <c r="E43" t="n">
+        <v>7.736580771530863</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>REGN</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0.008583980147180573</v>
+      </c>
+      <c r="C44" t="n">
+        <v>725.3400268554688</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1028.345816834935</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1.417743098079218</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>VLO</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0.008277317609489345</v>
+      </c>
+      <c r="C45" t="n">
+        <v>185.4299926757812</v>
+      </c>
+      <c r="D45" t="n">
+        <v>991.6081808656421</v>
+      </c>
+      <c r="E45" t="n">
+        <v>5.347614841356539</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>JNJ</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0.008084432907643057</v>
+      </c>
+      <c r="C46" t="n">
+        <v>200</v>
+      </c>
+      <c r="D46" t="n">
+        <v>968.5009307469156</v>
+      </c>
+      <c r="E46" t="n">
+        <v>4.842504653734578</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0.007473288376255044</v>
+      </c>
+      <c r="C47" t="n">
+        <v>92.83000183105469</v>
+      </c>
+      <c r="D47" t="n">
+        <v>895.2868841672725</v>
+      </c>
+      <c r="E47" t="n">
+        <v>9.644369993621714</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>HPE</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0.007471235114235881</v>
+      </c>
+      <c r="C48" t="n">
+        <v>20.89999961853027</v>
+      </c>
+      <c r="D48" t="n">
+        <v>895.0409069664788</v>
+      </c>
+      <c r="E48" t="n">
+        <v>42.82492455994694</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>WBD</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0.007090181884668373</v>
+      </c>
+      <c r="C49" t="n">
+        <v>23.69000053405762</v>
+      </c>
+      <c r="D49" t="n">
+        <v>849.3913961453367</v>
+      </c>
+      <c r="E49" t="n">
+        <v>35.85442705770396</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>FOXA</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>0.00677893541549476</v>
+      </c>
+      <c r="C50" t="n">
+        <v>64.95999908447266</v>
+      </c>
+      <c r="D50" t="n">
+        <v>812.1046131971659</v>
+      </c>
+      <c r="E50" t="n">
+        <v>12.50161060102728</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>HSIC</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>0.006751975328029743</v>
+      </c>
+      <c r="C51" t="n">
+        <v>71.19999694824219</v>
+      </c>
+      <c r="D51" t="n">
+        <v>808.8748418450898</v>
+      </c>
+      <c r="E51" t="n">
+        <v>11.36060219824293</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>DVN</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>0.005774306525005767</v>
+      </c>
+      <c r="C52" t="n">
+        <v>35.86999893188477</v>
+      </c>
+      <c r="D52" t="n">
+        <v>691.7518282078852</v>
+      </c>
+      <c r="E52" t="n">
+        <v>19.28496930043085</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>ABBV</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>0.005759395305158078</v>
+      </c>
+      <c r="C53" t="n">
+        <v>233.8699951171875</v>
+      </c>
+      <c r="D53" t="n">
+        <v>689.9654901349443</v>
+      </c>
+      <c r="E53" t="n">
+        <v>2.950209537521975</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>HAL</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>0.005647868665337517</v>
+      </c>
+      <c r="C54" t="n">
+        <v>26.79000091552734</v>
+      </c>
+      <c r="D54" t="n">
+        <v>676.6047936330075</v>
+      </c>
+      <c r="E54" t="n">
+        <v>25.25587049311562</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>BG</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0.005642135857227075</v>
+      </c>
+      <c r="C55" t="n">
+        <v>96.13999938964844</v>
+      </c>
+      <c r="D55" t="n">
+        <v>675.9180132423252</v>
+      </c>
+      <c r="E55" t="n">
+        <v>7.030559782956504</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>GILD</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>0.005330090176685706</v>
+      </c>
+      <c r="C56" t="n">
+        <v>127.1800003051758</v>
+      </c>
+      <c r="D56" t="n">
+        <v>638.5354861693187</v>
+      </c>
+      <c r="E56" t="n">
+        <v>5.020722477096365</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>0.005288061552762281</v>
+      </c>
+      <c r="C57" t="n">
+        <v>13.02000045776367</v>
+      </c>
+      <c r="D57" t="n">
+        <v>633.500530489327</v>
+      </c>
+      <c r="E57" t="n">
+        <v>48.65595301201224</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>CSCO</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>0.005197399085282128</v>
+      </c>
+      <c r="C58" t="n">
+        <v>77.37000274658203</v>
+      </c>
+      <c r="D58" t="n">
+        <v>622.6393253631978</v>
+      </c>
+      <c r="E58" t="n">
+        <v>8.047554649863368</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>TER</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>0.004990379988500426</v>
+      </c>
+      <c r="C59" t="n">
+        <v>163.7200012207031</v>
+      </c>
+      <c r="D59" t="n">
+        <v>597.8387994381311</v>
+      </c>
+      <c r="E59" t="n">
+        <v>3.651592932938066</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>ROK</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>0.004927277872716004</v>
+      </c>
+      <c r="C60" t="n">
+        <v>366.010009765625</v>
+      </c>
+      <c r="D60" t="n">
+        <v>590.2792762696557</v>
+      </c>
+      <c r="E60" t="n">
+        <v>1.612740800853075</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>ALB</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>0.004894196494618075</v>
+      </c>
+      <c r="C61" t="n">
+        <v>121.3899993896484</v>
+      </c>
+      <c r="D61" t="n">
+        <v>586.3161849997728</v>
+      </c>
+      <c r="E61" t="n">
+        <v>4.830020495492078</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>IQV</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>0.004893072348490434</v>
+      </c>
+      <c r="C62" t="n">
+        <v>217.2799987792969</v>
+      </c>
+      <c r="D62" t="n">
+        <v>586.1815142586888</v>
+      </c>
+      <c r="E62" t="n">
+        <v>2.697816262665324</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>STX</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>0.004878770527820644</v>
+      </c>
+      <c r="C63" t="n">
+        <v>253.8600006103516</v>
+      </c>
+      <c r="D63" t="n">
+        <v>584.4681811420305</v>
+      </c>
+      <c r="E63" t="n">
+        <v>2.302324823669751</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>FOX</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>0.004530461899621269</v>
+      </c>
+      <c r="C64" t="n">
+        <v>58.52000045776367</v>
+      </c>
+      <c r="D64" t="n">
+        <v>542.7414163272275</v>
+      </c>
+      <c r="E64" t="n">
+        <v>9.274460220125027</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>NEE</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>0.004109679827306444</v>
+      </c>
+      <c r="C65" t="n">
+        <v>84.63999938964844</v>
+      </c>
+      <c r="D65" t="n">
+        <v>492.3324595909738</v>
+      </c>
+      <c r="E65" t="n">
+        <v>5.816782409513894</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>FICO</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0.003668131995651883</v>
+      </c>
+      <c r="C66" t="n">
+        <v>1724.969970703125</v>
+      </c>
+      <c r="D66" t="n">
+        <v>439.4358011843672</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.2547498267493006</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>AIZ</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0.00355263170585966</v>
+      </c>
+      <c r="C67" t="n">
+        <v>225.9499969482422</v>
+      </c>
+      <c r="D67" t="n">
+        <v>425.5990683617654</v>
+      </c>
+      <c r="E67" t="n">
+        <v>1.883598469174825</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>FSLR</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>0.003382617269823928</v>
+      </c>
+      <c r="C68" t="n">
+        <v>252.1900024414062</v>
+      </c>
+      <c r="D68" t="n">
+        <v>405.231636109919</v>
+      </c>
+      <c r="E68" t="n">
+        <v>1.606850518208272</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>APA</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>0.003108359639444114</v>
+      </c>
+      <c r="C69" t="n">
+        <v>24.92000007629395</v>
+      </c>
+      <c r="D69" t="n">
+        <v>372.3760513927551</v>
+      </c>
+      <c r="E69" t="n">
+        <v>14.94285915941836</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>VRTX</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>0.002946014797892389</v>
+      </c>
+      <c r="C70" t="n">
+        <v>435.5199890136719</v>
+      </c>
+      <c r="D70" t="n">
+        <v>352.9274231536414</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.8103587253318063</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>VTRS</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>0.002834765995548434</v>
+      </c>
+      <c r="C71" t="n">
+        <v>10.71000003814697</v>
+      </c>
+      <c r="D71" t="n">
+        <v>339.6000110957422</v>
+      </c>
+      <c r="E71" t="n">
+        <v>31.70868439646609</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>SOLV</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>0.002827548604195691</v>
+      </c>
+      <c r="C72" t="n">
+        <v>76.88999938964844</v>
+      </c>
+      <c r="D72" t="n">
+        <v>338.7353802276837</v>
+      </c>
+      <c r="E72" t="n">
+        <v>4.405454323274283</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>HII</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>0.002732727519724341</v>
+      </c>
+      <c r="C73" t="n">
+        <v>309.1600036621094</v>
+      </c>
+      <c r="D73" t="n">
+        <v>327.3759800552716</v>
+      </c>
+      <c r="E73" t="n">
+        <v>1.058920870026483</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>TRGP</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>0.002579774954349508</v>
+      </c>
+      <c r="C74" t="n">
+        <v>169.5800018310547</v>
+      </c>
+      <c r="D74" t="n">
+        <v>309.0525300844509</v>
+      </c>
+      <c r="E74" t="n">
+        <v>1.822458584428763</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>STE</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>0.002434842217869821</v>
+      </c>
+      <c r="C75" t="n">
+        <v>257</v>
+      </c>
+      <c r="D75" t="n">
+        <v>291.6898415966077</v>
+      </c>
+      <c r="E75" t="n">
+        <v>1.13497992839147</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>NUE</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>0.001557195232112158</v>
+      </c>
+      <c r="C76" t="n">
+        <v>148.5099945068359</v>
+      </c>
+      <c r="D76" t="n">
+        <v>186.5492668297708</v>
+      </c>
+      <c r="E76" t="n">
+        <v>1.256139477004586</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>AVGO</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>0.001430738557402473</v>
+      </c>
+      <c r="C77" t="n">
+        <v>340.5</v>
+      </c>
+      <c r="D77" t="n">
+        <v>171.3999782458179</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.5033773223078352</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>KDP</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>0.00113196301235232</v>
+      </c>
+      <c r="C78" t="n">
+        <v>27.42000007629395</v>
+      </c>
+      <c r="D78" t="n">
+        <v>135.6071902084624</v>
+      </c>
+      <c r="E78" t="n">
+        <v>4.945557616015545</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>STLD</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>0.0002655789412208195</v>
+      </c>
+      <c r="C79" t="n">
+        <v>154.6100006103516</v>
+      </c>
+      <c r="D79" t="n">
+        <v>31.81589292626492</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.2057815975723808</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>DLTR</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>0.0002487894377271578</v>
+      </c>
+      <c r="C80" t="n">
+        <v>101.5699996948242</v>
+      </c>
+      <c r="D80" t="n">
+        <v>29.80453975577636</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.2934384153325456</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G80"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Shares</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Entry_Price</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Exit_Price</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Sale_Value</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>Transaction_Cost</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>Gain_Loss</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CAH</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>32.38663173328271</v>
+      </c>
+      <c r="C2" t="n">
+        <v>206.9700012207031</v>
+      </c>
+      <c r="D2" t="n">
+        <v>207.5200042724609</v>
+      </c>
+      <c r="E2" t="n">
+        <v>6720.873955661446</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>17.81274628946176</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>COR</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>17.98400353527994</v>
+      </c>
+      <c r="C3" t="n">
+        <v>361.6400146484375</v>
+      </c>
+      <c r="D3" t="n">
+        <v>360.7300109863281</v>
+      </c>
+      <c r="E3" t="n">
+        <v>6487.369792859698</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-16.36550907649234</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>DD</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>134.2240591921018</v>
+      </c>
+      <c r="C4" t="n">
+        <v>38.70000076293945</v>
+      </c>
+      <c r="D4" t="n">
+        <v>37.88000106811523</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5084.407505563579</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-110.0636875755918</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>WELL</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>20.36320620903575</v>
+      </c>
+      <c r="C5" t="n">
+        <v>198.2899932861328</v>
+      </c>
+      <c r="D5" t="n">
+        <v>196.8999938964844</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4009.515178271992</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-28.3048442018453</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>INCY</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>33.1015484326355</v>
+      </c>
+      <c r="C6" t="n">
+        <v>103.8899993896484</v>
+      </c>
+      <c r="D6" t="n">
+        <v>101.3199996948242</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3353.848877092837</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-85.07096937008237</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>VTR</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>42.83620122707109</v>
+      </c>
+      <c r="C7" t="n">
+        <v>79.86000061035156</v>
+      </c>
+      <c r="D7" t="n">
+        <v>80</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3426.896098165687</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>5.997042026647705</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>AEP</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>26.68262017499511</v>
+      </c>
+      <c r="C8" t="n">
+        <v>123.5100021362305</v>
+      </c>
+      <c r="D8" t="n">
+        <v>121.7099990844727</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3247.541677069987</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-48.02879774388566</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>EXPD</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>22.59900607639895</v>
+      </c>
+      <c r="C9" t="n">
+        <v>139.9100036621094</v>
+      </c>
+      <c r="D9" t="n">
+        <v>139.1300048828125</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3144.199825756095</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-17.6271971529136</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>MCK</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>3.54582478683787</v>
+      </c>
+      <c r="C10" t="n">
+        <v>860.75</v>
+      </c>
+      <c r="D10" t="n">
+        <v>852.469970703125</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3022.709152154093</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-29.35953311660296</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>AKAM</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>31.6662184080762</v>
+      </c>
+      <c r="C11" t="n">
+        <v>87.73999786376953</v>
+      </c>
+      <c r="D11" t="n">
+        <v>86.51999664306641</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2739.761110365361</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-38.63282511290481</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>HCA</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>5.675101706879875</v>
+      </c>
+      <c r="C12" t="n">
+        <v>478.1400146484375</v>
+      </c>
+      <c r="D12" t="n">
+        <v>481.0599975585938</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2730.064413256404</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>16.57119999748784</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>LVS</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>40.66644193690993</v>
+      </c>
+      <c r="C13" t="n">
+        <v>64.77999877929688</v>
+      </c>
+      <c r="D13" t="n">
+        <v>64.05000305175781</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2604.685730163213</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>-29.68632886815976</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>LLY</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2.434636921483844</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1030.050048828125</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1049.599975585938</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2555.394853350064</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>47.59697349687531</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>WDC</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>14.42568521524682</v>
+      </c>
+      <c r="C15" t="n">
+        <v>152.8600006103516</v>
+      </c>
+      <c r="D15" t="n">
+        <v>153.9700012207031</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2221.122770201032</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>16.0125193936633</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>AMGN</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>6.359704560607165</v>
+      </c>
+      <c r="C16" t="n">
+        <v>343.989990234375</v>
+      </c>
+      <c r="D16" t="n">
+        <v>342.3999938964844</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2177.562802735337</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>-10.11190696143149</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>CTRA</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>82.56544142807964</v>
+      </c>
+      <c r="C17" t="n">
+        <v>26.17000007629395</v>
+      </c>
+      <c r="D17" t="n">
+        <v>25.76000022888184</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2126.885790085061</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>-33.85181838702601</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>EPAM</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>11.22913432891134</v>
+      </c>
+      <c r="C18" t="n">
+        <v>178.7100067138672</v>
+      </c>
+      <c r="D18" t="n">
+        <v>180.9299926757812</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2031.687191885292</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>24.92852057463028</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>UHS</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>8.707861717265208</v>
+      </c>
+      <c r="C19" t="n">
+        <v>228.8399963378906</v>
+      </c>
+      <c r="D19" t="n">
+        <v>227.9400024414062</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1984.87002109286</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>-7.837022396968678</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>EW</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>23.38124594548207</v>
+      </c>
+      <c r="C20" t="n">
+        <v>84.04000091552734</v>
+      </c>
+      <c r="D20" t="n">
+        <v>86.01999664306641</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2011.254697741078</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>46.29476707659455</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>6.818594623902554</v>
+      </c>
+      <c r="C21" t="n">
+        <v>284.2799987792969</v>
+      </c>
+      <c r="D21" t="n">
+        <v>292.8099975585938</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1996.552675177947</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>58.1626038184088</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>ISRG</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>3.530140143041185</v>
+      </c>
+      <c r="C22" t="n">
+        <v>546.77001953125</v>
+      </c>
+      <c r="D22" t="n">
+        <v>564.6400146484375</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1993.258382077812</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>63.08358711913343</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>DDOG</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>10.8383038236993</v>
+      </c>
+      <c r="C23" t="n">
+        <v>176.4600067138672</v>
+      </c>
+      <c r="D23" t="n">
+        <v>176.3099975585938</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1910.90132069572</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>-1.625844801190169</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>6.581630253809045</v>
+      </c>
+      <c r="C24" t="n">
+        <v>284.9599914550781</v>
+      </c>
+      <c r="D24" t="n">
+        <v>292.989990234375</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1928.351783789779</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>52.85048290387022</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>MU</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>8.202287224479758</v>
+      </c>
+      <c r="C25" t="n">
+        <v>228.5</v>
+      </c>
+      <c r="D25" t="n">
+        <v>225.9199981689453</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1853.06071473563</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>-21.16191605799418</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>2.241411288187976</v>
+      </c>
+      <c r="C26" t="n">
+        <v>817.2999877929688</v>
+      </c>
+      <c r="D26" t="n">
+        <v>820.6699829101562</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1839.458963571858</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>7.553545096802509</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>CMI</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>3.913274563594206</v>
+      </c>
+      <c r="C27" t="n">
+        <v>464.9200134277344</v>
+      </c>
+      <c r="D27" t="n">
+        <v>473.260009765625</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1851.996358182166</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>32.63669552953615</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>3.303823691325687</v>
+      </c>
+      <c r="C28" t="n">
+        <v>546.8800048828125</v>
+      </c>
+      <c r="D28" t="n">
+        <v>553.1099853515625</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1827.377873513296</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>20.58275706915242</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>PFE</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>70.43931853245313</v>
+      </c>
+      <c r="C29" t="n">
+        <v>25.45000076293945</v>
+      </c>
+      <c r="D29" t="n">
+        <v>24.8799991607666</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1752.530185972405</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>-40.15052441946204</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>EQT</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>29.764669068969</v>
+      </c>
+      <c r="C30" t="n">
+        <v>58.75</v>
+      </c>
+      <c r="D30" t="n">
+        <v>58.88999938964844</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1752.841343304672</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>4.167035502743374</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>FDS</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>6.190288543789459</v>
+      </c>
+      <c r="C31" t="n">
+        <v>272.1099853515625</v>
+      </c>
+      <c r="D31" t="n">
+        <v>267.0199890136719</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1652.93077895412</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>-31.50854601837455</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>FDX</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>6.380674933678142</v>
+      </c>
+      <c r="C32" t="n">
+        <v>263.0799865722656</v>
+      </c>
+      <c r="D32" t="n">
+        <v>262.5700073242188</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1675.373864069329</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>-3.254011804708853</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>4.451173415018875</v>
+      </c>
+      <c r="C33" t="n">
+        <v>376.6300048828125</v>
+      </c>
+      <c r="D33" t="n">
+        <v>376.25</v>
+      </c>
+      <c r="E33" t="n">
+        <v>1674.753997400852</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>-1.691467631952264</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>ES</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>22.48269379422383</v>
+      </c>
+      <c r="C34" t="n">
+        <v>74.54000091552734</v>
+      </c>
+      <c r="D34" t="n">
+        <v>65.26000213623047</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1467.220645039263</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>-208.6393709657025</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>EXE</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>14.24224509791294</v>
+      </c>
+      <c r="C35" t="n">
+        <v>117.1600036621094</v>
+      </c>
+      <c r="D35" t="n">
+        <v>117.2699966430664</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1670.188034821979</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1.56654699384012</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>DHR</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>6.93816335712723</v>
+      </c>
+      <c r="C36" t="n">
+        <v>225.5099945068359</v>
+      </c>
+      <c r="D36" t="n">
+        <v>222.4100036621094</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1543.11693766698</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>-21.50824288631156</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>JKHY</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>9.018498623326296</v>
+      </c>
+      <c r="C37" t="n">
+        <v>163.9400024414062</v>
+      </c>
+      <c r="D37" t="n">
+        <v>165.8000030517578</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1495.267099269774</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>16.77441294384153</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>MAR</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>5.088678325444903</v>
+      </c>
+      <c r="C38" t="n">
+        <v>282.8999938964844</v>
+      </c>
+      <c r="D38" t="n">
+        <v>284.2000122070312</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1446.202442209097</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>6.615374999561482</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>TMO</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>2.486957674779311</v>
+      </c>
+      <c r="C39" t="n">
+        <v>576.030029296875</v>
+      </c>
+      <c r="D39" t="n">
+        <v>573.7899780273438</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1426.991389566555</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>-5.570912696659889</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>EXPE</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>5.731748132888083</v>
+      </c>
+      <c r="C40" t="n">
+        <v>239.6000061035156</v>
+      </c>
+      <c r="D40" t="n">
+        <v>239.9600067138672</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1375.39032045002</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>2.063432826221288</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>18.27680774374096</v>
+      </c>
+      <c r="C41" t="n">
+        <v>67.93000030517578</v>
+      </c>
+      <c r="D41" t="n">
+        <v>68.5</v>
+      </c>
+      <c r="E41" t="n">
+        <v>1251.961330446256</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>10.41777483629312</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>BIIB</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>7.134522456985254</v>
+      </c>
+      <c r="C42" t="n">
+        <v>168.8300018310547</v>
+      </c>
+      <c r="D42" t="n">
+        <v>167.9299926757812</v>
+      </c>
+      <c r="E42" t="n">
+        <v>1198.10030394673</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>-6.421135529790718</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>CHRW</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>7.736580771530863</v>
+      </c>
+      <c r="C43" t="n">
+        <v>151.6900024414062</v>
+      </c>
+      <c r="D43" t="n">
+        <v>151.3600006103516</v>
+      </c>
+      <c r="E43" t="n">
+        <v>1171.008870300946</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>-2.553085820707793</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>REGN</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>1.417743098079218</v>
+      </c>
+      <c r="C44" t="n">
+        <v>725.3400268554688</v>
+      </c>
+      <c r="D44" t="n">
+        <v>702.75</v>
+      </c>
+      <c r="E44" t="n">
+        <v>996.3189621751702</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>-32.02685465976504</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>VLO</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>5.347614841356539</v>
+      </c>
+      <c r="C45" t="n">
+        <v>185.4299926757812</v>
+      </c>
+      <c r="D45" t="n">
+        <v>180.3300018310547</v>
+      </c>
+      <c r="E45" t="n">
+        <v>964.3353941335999</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>-27.27278673204228</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>JNJ</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>4.842504653734578</v>
+      </c>
+      <c r="C46" t="n">
+        <v>200</v>
+      </c>
+      <c r="D46" t="n">
+        <v>202.5099945068359</v>
+      </c>
+      <c r="E46" t="n">
+        <v>980.655590827117</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>12.15466008020132</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>9.644369993621714</v>
+      </c>
+      <c r="C47" t="n">
+        <v>92.83000183105469</v>
+      </c>
+      <c r="D47" t="n">
+        <v>92.41000366210938</v>
+      </c>
+      <c r="E47" t="n">
+        <v>891.2362664293204</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>-4.050617737952166</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>HPE</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>42.82492455994694</v>
+      </c>
+      <c r="C48" t="n">
+        <v>20.89999961853027</v>
+      </c>
+      <c r="D48" t="n">
+        <v>20.60000038146973</v>
+      </c>
+      <c r="E48" t="n">
+        <v>882.1934622713193</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>-12.84744469515954</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>WBD</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>35.85442705770396</v>
+      </c>
+      <c r="C49" t="n">
+        <v>23.69000053405762</v>
+      </c>
+      <c r="D49" t="n">
+        <v>23.09000015258789</v>
+      </c>
+      <c r="E49" t="n">
+        <v>827.8787262333358</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>-21.51266991200089</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>FOXA</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>12.50161060102728</v>
+      </c>
+      <c r="C50" t="n">
+        <v>64.95999908447266</v>
+      </c>
+      <c r="D50" t="n">
+        <v>64.77999877929688</v>
+      </c>
+      <c r="E50" t="n">
+        <v>809.8543194737922</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>-2.250293723373716</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>HSIC</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>11.36060219824293</v>
+      </c>
+      <c r="C51" t="n">
+        <v>71.19999694824219</v>
+      </c>
+      <c r="D51" t="n">
+        <v>70.59999847412109</v>
+      </c>
+      <c r="E51" t="n">
+        <v>802.0584978610474</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>-6.816343984042419</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>DVN</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>19.28496930043085</v>
+      </c>
+      <c r="C52" t="n">
+        <v>35.86999893188477</v>
+      </c>
+      <c r="D52" t="n">
+        <v>35.27999877929688</v>
+      </c>
+      <c r="E52" t="n">
+        <v>680.3736933779782</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="n">
+        <v>-11.37813482990703</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>ABBV</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>2.950209537521975</v>
+      </c>
+      <c r="C53" t="n">
+        <v>233.8699951171875</v>
+      </c>
+      <c r="D53" t="n">
+        <v>232.9100036621094</v>
+      </c>
+      <c r="E53" t="n">
+        <v>687.1333141882332</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" t="n">
+        <v>-2.832175946711118</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>HAL</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>25.25587049311562</v>
+      </c>
+      <c r="C54" t="n">
+        <v>26.79000091552734</v>
+      </c>
+      <c r="D54" t="n">
+        <v>26.45999908447266</v>
+      </c>
+      <c r="E54" t="n">
+        <v>668.2703101253993</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="n">
+        <v>-8.334483507608184</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>BG</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>7.030559782956504</v>
+      </c>
+      <c r="C55" t="n">
+        <v>96.13999938964844</v>
+      </c>
+      <c r="D55" t="n">
+        <v>93.15000152587891</v>
+      </c>
+      <c r="E55" t="n">
+        <v>654.8966545101813</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" t="n">
+        <v>-21.02135873214388</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>GILD</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>5.020722477096365</v>
+      </c>
+      <c r="C56" t="n">
+        <v>127.1800003051758</v>
+      </c>
+      <c r="D56" t="n">
+        <v>128.0700073242188</v>
+      </c>
+      <c r="E56" t="n">
+        <v>643.0039644146012</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" t="n">
+        <v>4.46847824528254</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>48.65595301201224</v>
+      </c>
+      <c r="C57" t="n">
+        <v>13.02000045776367</v>
+      </c>
+      <c r="D57" t="n">
+        <v>12.89999961853027</v>
+      </c>
+      <c r="E57" t="n">
+        <v>627.6617752941848</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" t="n">
+        <v>-5.838755195142198</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>CSCO</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>8.047554649863368</v>
+      </c>
+      <c r="C58" t="n">
+        <v>77.37000274658203</v>
+      </c>
+      <c r="D58" t="n">
+        <v>78.38999938964844</v>
+      </c>
+      <c r="E58" t="n">
+        <v>630.8478040909519</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" t="n">
+        <v>8.208478727754027</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>TER</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>3.651592932938066</v>
+      </c>
+      <c r="C59" t="n">
+        <v>163.7200012207031</v>
+      </c>
+      <c r="D59" t="n">
+        <v>168.2299957275391</v>
+      </c>
+      <c r="E59" t="n">
+        <v>614.3074635068828</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" t="n">
+        <v>16.46866406875165</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>ROK</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>1.612740800853075</v>
+      </c>
+      <c r="C60" t="n">
+        <v>366.010009765625</v>
+      </c>
+      <c r="D60" t="n">
+        <v>372.4800109863281</v>
+      </c>
+      <c r="E60" t="n">
+        <v>600.7137112198528</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" t="n">
+        <v>10.4344349501971</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>ALB</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>4.830020495492078</v>
+      </c>
+      <c r="C61" t="n">
+        <v>121.3899993896484</v>
+      </c>
+      <c r="D61" t="n">
+        <v>125.6800003051758</v>
+      </c>
+      <c r="E61" t="n">
+        <v>607.0369773474496</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="n">
+        <v>20.72079234767682</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>IQV</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>2.697816262665324</v>
+      </c>
+      <c r="C62" t="n">
+        <v>217.2799987792969</v>
+      </c>
+      <c r="D62" t="n">
+        <v>217.4799957275391</v>
+      </c>
+      <c r="E62" t="n">
+        <v>586.72106927814</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.5395550194511998</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>STX</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>2.302324823669751</v>
+      </c>
+      <c r="C63" t="n">
+        <v>253.8600006103516</v>
+      </c>
+      <c r="D63" t="n">
+        <v>259.1400146484375</v>
+      </c>
+      <c r="E63" t="n">
+        <v>596.6244885312406</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0</v>
+      </c>
+      <c r="G63" t="n">
+        <v>12.15630738921004</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>FOX</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>9.274460220125027</v>
+      </c>
+      <c r="C64" t="n">
+        <v>58.52000045776367</v>
+      </c>
+      <c r="D64" t="n">
+        <v>58.2599983215332</v>
+      </c>
+      <c r="E64" t="n">
+        <v>540.3300368576105</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G64" t="n">
+        <v>-2.411379469617032</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>NEE</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>5.816782409513894</v>
+      </c>
+      <c r="C65" t="n">
+        <v>84.63999938964844</v>
+      </c>
+      <c r="D65" t="n">
+        <v>84.26999664306641</v>
+      </c>
+      <c r="E65" t="n">
+        <v>490.1802341231835</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0</v>
+      </c>
+      <c r="G65" t="n">
+        <v>-2.152225467790174</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>FICO</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0.2547498267493006</v>
+      </c>
+      <c r="C66" t="n">
+        <v>1724.969970703125</v>
+      </c>
+      <c r="D66" t="n">
+        <v>1736.160034179688</v>
+      </c>
+      <c r="E66" t="n">
+        <v>442.2864679163351</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" t="n">
+        <v>2.850666731967976</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>AIZ</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>1.883598469174825</v>
+      </c>
+      <c r="C67" t="n">
+        <v>225.9499969482422</v>
+      </c>
+      <c r="D67" t="n">
+        <v>224.6199951171875</v>
+      </c>
+      <c r="E67" t="n">
+        <v>423.0938789487911</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0</v>
+      </c>
+      <c r="G67" t="n">
+        <v>-2.505189412974289</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>FSLR</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>1.606850518208272</v>
+      </c>
+      <c r="C68" t="n">
+        <v>252.1900024414062</v>
+      </c>
+      <c r="D68" t="n">
+        <v>251.8699951171875</v>
+      </c>
+      <c r="E68" t="n">
+        <v>404.7174321751676</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" t="n">
+        <v>-0.5142039347513219</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>APA</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>14.94285915941836</v>
+      </c>
+      <c r="C69" t="n">
+        <v>24.92000007629395</v>
+      </c>
+      <c r="D69" t="n">
+        <v>24.04999923706055</v>
+      </c>
+      <c r="E69" t="n">
+        <v>359.3757513835147</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0</v>
+      </c>
+      <c r="G69" t="n">
+        <v>-13.00030000924045</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>VRTX</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>0.8103587253318063</v>
+      </c>
+      <c r="C70" t="n">
+        <v>435.5199890136719</v>
+      </c>
+      <c r="D70" t="n">
+        <v>421.0299987792969</v>
+      </c>
+      <c r="E70" t="n">
+        <v>341.185333137243</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" t="n">
+        <v>-11.74209001639844</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>VTRS</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>31.70868439646609</v>
+      </c>
+      <c r="C71" t="n">
+        <v>10.71000003814697</v>
+      </c>
+      <c r="D71" t="n">
+        <v>10.46000003814697</v>
+      </c>
+      <c r="E71" t="n">
+        <v>331.6728399966257</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" t="n">
+        <v>-7.927171099116492</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>SOLV</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>4.405454323274283</v>
+      </c>
+      <c r="C72" t="n">
+        <v>76.88999938964844</v>
+      </c>
+      <c r="D72" t="n">
+        <v>77.30999755859375</v>
+      </c>
+      <c r="E72" t="n">
+        <v>340.5856629768311</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0</v>
+      </c>
+      <c r="G72" t="n">
+        <v>1.850282749147425</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>HII</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>1.058920870026483</v>
+      </c>
+      <c r="C73" t="n">
+        <v>309.1600036621094</v>
+      </c>
+      <c r="D73" t="n">
+        <v>309.739990234375</v>
+      </c>
+      <c r="E73" t="n">
+        <v>327.9901399409788</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0.6141598857072381</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>TRGP</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>1.822458584428763</v>
+      </c>
+      <c r="C74" t="n">
+        <v>169.5800018310547</v>
+      </c>
+      <c r="D74" t="n">
+        <v>170.1600036621094</v>
+      </c>
+      <c r="E74" t="n">
+        <v>310.1095594004409</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" t="n">
+        <v>1.057029315990007</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>STE</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>1.13497992839147</v>
+      </c>
+      <c r="C75" t="n">
+        <v>257</v>
+      </c>
+      <c r="D75" t="n">
+        <v>254.7100067138672</v>
+      </c>
+      <c r="E75" t="n">
+        <v>289.0907451806958</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0</v>
+      </c>
+      <c r="G75" t="n">
+        <v>-2.599096415911959</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>NUE</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>1.256139477004586</v>
+      </c>
+      <c r="C76" t="n">
+        <v>148.5099945068359</v>
+      </c>
+      <c r="D76" t="n">
+        <v>148.5800018310547</v>
+      </c>
+      <c r="E76" t="n">
+        <v>186.6372057934014</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0.08793896363062004</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>AVGO</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>0.5033773223078352</v>
+      </c>
+      <c r="C77" t="n">
+        <v>340.5</v>
+      </c>
+      <c r="D77" t="n">
+        <v>354.4200134277344</v>
+      </c>
+      <c r="E77" t="n">
+        <v>178.4069973315599</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0</v>
+      </c>
+      <c r="G77" t="n">
+        <v>7.007019085742058</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>KDP</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>4.945557616015545</v>
+      </c>
+      <c r="C78" t="n">
+        <v>27.42000007629395</v>
+      </c>
+      <c r="D78" t="n">
+        <v>26.88999938964844</v>
+      </c>
+      <c r="E78" t="n">
+        <v>132.9860412761292</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0</v>
+      </c>
+      <c r="G78" t="n">
+        <v>-2.62114893233317</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>STLD</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>0.2057815975723808</v>
+      </c>
+      <c r="C79" t="n">
+        <v>154.6100006103516</v>
+      </c>
+      <c r="D79" t="n">
+        <v>155.4600067138672</v>
+      </c>
+      <c r="E79" t="n">
+        <v>31.99080854019264</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0</v>
+      </c>
+      <c r="G79" t="n">
+        <v>0.1749156139277197</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>DLTR</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>0.2934384153325456</v>
+      </c>
+      <c r="C80" t="n">
+        <v>101.5699996948242</v>
+      </c>
+      <c r="D80" t="n">
+        <v>99.94999694824219</v>
+      </c>
+      <c r="E80" t="n">
+        <v>29.32916871698496</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0</v>
+      </c>
+      <c r="G80" t="n">
+        <v>-0.4753710387914047</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
need to commit before switch branch for testing
</commit_message>
<xml_diff>
--- a/backtest_portfolio_PL.xlsx
+++ b/backtest_portfolio_PL.xlsx
@@ -52,6 +52,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="11-20-2025_PnL" sheetId="44" state="visible" r:id="rId44"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="11-21-2025_Allocations" sheetId="45" state="visible" r:id="rId45"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="11-21-2025_PnL" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="11-24-2025_Allocations" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="11-24-2025_PnL" sheetId="48" state="visible" r:id="rId48"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -82625,6 +82627,3628 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E81"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Allocation_Percent</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Entry_Price</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Target_Value</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Actual_Shares</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>WELL</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.04731608229890785</v>
+      </c>
+      <c r="C2" t="n">
+        <v>199.9299926757812</v>
+      </c>
+      <c r="D2" t="n">
+        <v>5664.643519959408</v>
+      </c>
+      <c r="E2" t="n">
+        <v>28.33313523471959</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CAH</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.04729167916041049</v>
+      </c>
+      <c r="C3" t="n">
+        <v>209.4799957275391</v>
+      </c>
+      <c r="D3" t="n">
+        <v>5661.721995741015</v>
+      </c>
+      <c r="E3" t="n">
+        <v>27.02750673675283</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>COR</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.03979123318317224</v>
+      </c>
+      <c r="C4" t="n">
+        <v>365.6799926757812</v>
+      </c>
+      <c r="D4" t="n">
+        <v>4763.774603702835</v>
+      </c>
+      <c r="E4" t="n">
+        <v>13.02716773987273</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>HCA</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.03351838777113571</v>
+      </c>
+      <c r="C5" t="n">
+        <v>491</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4012.79456925015</v>
+      </c>
+      <c r="E5" t="n">
+        <v>8.172697697047148</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>VTR</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.03303860184401431</v>
+      </c>
+      <c r="C6" t="n">
+        <v>79.23999786376953</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3955.354981883918</v>
+      </c>
+      <c r="E6" t="n">
+        <v>49.91614195502652</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MCK</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.02938871475045215</v>
+      </c>
+      <c r="C7" t="n">
+        <v>866.030029296875</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3518.393418952331</v>
+      </c>
+      <c r="E7" t="n">
+        <v>4.062669076046815</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>LLY</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.02866463922343617</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1059.699951171875</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3431.707676118399</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3.238376742702901</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>EXPD</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.02752964566560955</v>
+      </c>
+      <c r="C9" t="n">
+        <v>143.2100067138672</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3295.827155370243</v>
+      </c>
+      <c r="E9" t="n">
+        <v>23.01394456293329</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.0257390047823028</v>
+      </c>
+      <c r="C10" t="n">
+        <v>299.6499938964844</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3081.453061333465</v>
+      </c>
+      <c r="E10" t="n">
+        <v>10.28350783947611</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.02423963793102697</v>
+      </c>
+      <c r="C11" t="n">
+        <v>839.5700073242188</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2901.950061392204</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3.456471808278343</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.02414900601524342</v>
+      </c>
+      <c r="C12" t="n">
+        <v>299.6600036621094</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2891.09968094013</v>
+      </c>
+      <c r="E12" t="n">
+        <v>9.647933142923126</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>DHR</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.02283039526235367</v>
+      </c>
+      <c r="C13" t="n">
+        <v>227.3899993896484</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2733.236656492771</v>
+      </c>
+      <c r="E13" t="n">
+        <v>12.02003898073451</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>EXPE</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.02217094524688231</v>
+      </c>
+      <c r="C14" t="n">
+        <v>247.4900054931641</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2654.287828200553</v>
+      </c>
+      <c r="E14" t="n">
+        <v>10.72482835382161</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>CSCO</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.02162627294698436</v>
+      </c>
+      <c r="C15" t="n">
+        <v>76.09999847412109</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2589.080096194611</v>
+      </c>
+      <c r="E15" t="n">
+        <v>34.02207816173695</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.0206885515142665</v>
+      </c>
+      <c r="C16" t="n">
+        <v>393.989990234375</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2476.816836446774</v>
+      </c>
+      <c r="E16" t="n">
+        <v>6.286496859916102</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>FDS</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.01945552631794438</v>
+      </c>
+      <c r="C17" t="n">
+        <v>277.0199890136719</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2329.200046363246</v>
+      </c>
+      <c r="E17" t="n">
+        <v>8.408057680806175</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>DD</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.01937844561316976</v>
+      </c>
+      <c r="C18" t="n">
+        <v>38.54000091552734</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2319.972006052193</v>
+      </c>
+      <c r="E18" t="n">
+        <v>60.19646992580901</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.01772546896162612</v>
+      </c>
+      <c r="C19" t="n">
+        <v>94.66000366210938</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2122.07896371071</v>
+      </c>
+      <c r="E19" t="n">
+        <v>22.41790493993123</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>EPAM</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.01733845543203227</v>
+      </c>
+      <c r="C20" t="n">
+        <v>180.9799957275391</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2075.746013558557</v>
+      </c>
+      <c r="E20" t="n">
+        <v>11.4694776359899</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>AMGN</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0.0169225101902057</v>
+      </c>
+      <c r="C21" t="n">
+        <v>337.5400085449219</v>
+      </c>
+      <c r="D21" t="n">
+        <v>2025.949381963274</v>
+      </c>
+      <c r="E21" t="n">
+        <v>6.002101471457562</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>LVS</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.0167891120458536</v>
+      </c>
+      <c r="C22" t="n">
+        <v>64.30999755859375</v>
+      </c>
+      <c r="D22" t="n">
+        <v>2009.979062839957</v>
+      </c>
+      <c r="E22" t="n">
+        <v>31.25453489573897</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>ISRG</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.01657552756719168</v>
+      </c>
+      <c r="C23" t="n">
+        <v>561.6099853515625</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1984.408899922134</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3.533428805899726</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>AKAM</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.01636567924163963</v>
+      </c>
+      <c r="C24" t="n">
+        <v>89.01000213623047</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1959.286026265703</v>
+      </c>
+      <c r="E24" t="n">
+        <v>22.01197594925345</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>EW</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.01611633600641805</v>
+      </c>
+      <c r="C25" t="n">
+        <v>85.12999725341797</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1929.434853619564</v>
+      </c>
+      <c r="E25" t="n">
+        <v>22.66457084305964</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>CMI</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.01560124172725048</v>
+      </c>
+      <c r="C26" t="n">
+        <v>472.510009765625</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1867.768178593045</v>
+      </c>
+      <c r="E26" t="n">
+        <v>3.952864785911092</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>ROK</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0.01519964057890589</v>
+      </c>
+      <c r="C27" t="n">
+        <v>378.7300109863281</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1819.688810394149</v>
+      </c>
+      <c r="E27" t="n">
+        <v>4.804712480152092</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>TMO</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0.01498570739107161</v>
+      </c>
+      <c r="C28" t="n">
+        <v>587.47998046875</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1794.07690029318</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3.053851977835376</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>STE</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0.01466033560053068</v>
+      </c>
+      <c r="C29" t="n">
+        <v>263.2900085449219</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1755.123649827053</v>
+      </c>
+      <c r="E29" t="n">
+        <v>6.666123259013066</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>UHS</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0.01464996586101096</v>
+      </c>
+      <c r="C30" t="n">
+        <v>231.9199981689453</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1753.882192907544</v>
+      </c>
+      <c r="E30" t="n">
+        <v>7.562444837680207</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>HSIC</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0.0142633536152135</v>
+      </c>
+      <c r="C31" t="n">
+        <v>73.40000152587891</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1707.597284130468</v>
+      </c>
+      <c r="E31" t="n">
+        <v>23.26426769253423</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>FDX</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0.01420045357470954</v>
+      </c>
+      <c r="C32" t="n">
+        <v>269.4299926757812</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1700.066941601367</v>
+      </c>
+      <c r="E32" t="n">
+        <v>6.309865225907285</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>EXE</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.01403774102735497</v>
+      </c>
+      <c r="C33" t="n">
+        <v>114.9899978637695</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1680.587125602115</v>
+      </c>
+      <c r="E33" t="n">
+        <v>14.61507223952759</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>AEP</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.01329738277126456</v>
+      </c>
+      <c r="C34" t="n">
+        <v>120.8399963378906</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1591.952027469576</v>
+      </c>
+      <c r="E34" t="n">
+        <v>13.17404895493532</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>0.01324720734157749</v>
+      </c>
+      <c r="C35" t="n">
+        <v>151.25</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1585.945065167784</v>
+      </c>
+      <c r="E35" t="n">
+        <v>10.48558720772088</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>JKHY</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0.01311977685581704</v>
+      </c>
+      <c r="C36" t="n">
+        <v>170.8000030517578</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1570.689189356931</v>
+      </c>
+      <c r="E36" t="n">
+        <v>9.196072372908347</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>KDP</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0.01291272303694803</v>
+      </c>
+      <c r="C37" t="n">
+        <v>27.73999977111816</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1545.900871804988</v>
+      </c>
+      <c r="E37" t="n">
+        <v>55.72822222639387</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>MRK</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>0.0111048260267714</v>
+      </c>
+      <c r="C38" t="n">
+        <v>97.76000213623047</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1329.460888064251</v>
+      </c>
+      <c r="E38" t="n">
+        <v>13.59923137288419</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>REGN</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>0.0107963556020064</v>
+      </c>
+      <c r="C39" t="n">
+        <v>755.9000244140625</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1292.531055587724</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1.709923288585197</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>CB</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>0.0103352140954699</v>
+      </c>
+      <c r="C40" t="n">
+        <v>298.2900085449219</v>
+      </c>
+      <c r="D40" t="n">
+        <v>1237.32356333838</v>
+      </c>
+      <c r="E40" t="n">
+        <v>4.148055677004152</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>CTSH</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>0.01015518391785133</v>
+      </c>
+      <c r="C41" t="n">
+        <v>75.98000335693359</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1215.770494498027</v>
+      </c>
+      <c r="E41" t="n">
+        <v>16.0011903235469</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>IQV</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>0.009823154164687218</v>
+      </c>
+      <c r="C42" t="n">
+        <v>224.8999938964844</v>
+      </c>
+      <c r="D42" t="n">
+        <v>1176.020158073022</v>
+      </c>
+      <c r="E42" t="n">
+        <v>5.229080435699405</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>INCY</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>0.009026349763658178</v>
+      </c>
+      <c r="C43" t="n">
+        <v>102.0599975585938</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1080.627372625346</v>
+      </c>
+      <c r="E43" t="n">
+        <v>10.58815793136725</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>ABBV</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>0.009004370745076767</v>
+      </c>
+      <c r="C44" t="n">
+        <v>236.2799987792969</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1077.996062103995</v>
+      </c>
+      <c r="E44" t="n">
+        <v>4.562366970007153</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>DOV</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0.008470386474053003</v>
+      </c>
+      <c r="C45" t="n">
+        <v>183.5800018310547</v>
+      </c>
+      <c r="D45" t="n">
+        <v>1014.067892364446</v>
+      </c>
+      <c r="E45" t="n">
+        <v>5.523847272306242</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>BIIB</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0.008445602886882626</v>
+      </c>
+      <c r="C46" t="n">
+        <v>175.3000030517578</v>
+      </c>
+      <c r="D46" t="n">
+        <v>1011.100821135278</v>
+      </c>
+      <c r="E46" t="n">
+        <v>5.767831166761293</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0.007773313758832149</v>
+      </c>
+      <c r="C47" t="n">
+        <v>70.33000183105469</v>
+      </c>
+      <c r="D47" t="n">
+        <v>930.6149045563778</v>
+      </c>
+      <c r="E47" t="n">
+        <v>13.23211830410416</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>ALB</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0.007518002928674072</v>
+      </c>
+      <c r="C48" t="n">
+        <v>116.8199996948242</v>
+      </c>
+      <c r="D48" t="n">
+        <v>900.0492962185169</v>
+      </c>
+      <c r="E48" t="n">
+        <v>7.704582251068043</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>HIG</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0.007473247110958664</v>
+      </c>
+      <c r="C49" t="n">
+        <v>136.4499969482422</v>
+      </c>
+      <c r="D49" t="n">
+        <v>894.6911655262825</v>
+      </c>
+      <c r="E49" t="n">
+        <v>6.556915980479311</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>GILD</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>0.007264236082526511</v>
+      </c>
+      <c r="C50" t="n">
+        <v>126.6399993896484</v>
+      </c>
+      <c r="D50" t="n">
+        <v>869.6685324112078</v>
+      </c>
+      <c r="E50" t="n">
+        <v>6.867249973173125</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>CHRW</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>0.007148830035149751</v>
+      </c>
+      <c r="C51" t="n">
+        <v>151.6799926757812</v>
+      </c>
+      <c r="D51" t="n">
+        <v>855.8522127441</v>
+      </c>
+      <c r="E51" t="n">
+        <v>5.642485852260685</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>NUE</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>0.006892902535090344</v>
+      </c>
+      <c r="C52" t="n">
+        <v>152.3500061035156</v>
+      </c>
+      <c r="D52" t="n">
+        <v>825.2127771789878</v>
+      </c>
+      <c r="E52" t="n">
+        <v>5.416558871801353</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>STLD</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>0.006746812992624512</v>
+      </c>
+      <c r="C53" t="n">
+        <v>158.1600036621094</v>
+      </c>
+      <c r="D53" t="n">
+        <v>807.7230540266124</v>
+      </c>
+      <c r="E53" t="n">
+        <v>5.106999464619511</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>CTRA</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>0.006279609014688036</v>
+      </c>
+      <c r="C54" t="n">
+        <v>25.75</v>
+      </c>
+      <c r="D54" t="n">
+        <v>751.7897675512398</v>
+      </c>
+      <c r="E54" t="n">
+        <v>29.19571912820349</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>JBHT</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0.005463897272660892</v>
+      </c>
+      <c r="C55" t="n">
+        <v>166.4299926757812</v>
+      </c>
+      <c r="D55" t="n">
+        <v>654.1334103651438</v>
+      </c>
+      <c r="E55" t="n">
+        <v>3.93038177703611</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>0.005331649557774933</v>
+      </c>
+      <c r="C56" t="n">
+        <v>550.4299926757812</v>
+      </c>
+      <c r="D56" t="n">
+        <v>638.3008197371687</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1.159640332522988</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>FOXA</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>0.004937752898937272</v>
+      </c>
+      <c r="C57" t="n">
+        <v>65.69000244140625</v>
+      </c>
+      <c r="D57" t="n">
+        <v>591.143826858451</v>
+      </c>
+      <c r="E57" t="n">
+        <v>8.998992310675217</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>VTRS</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>0.004899361431639273</v>
+      </c>
+      <c r="C58" t="n">
+        <v>10.34000015258789</v>
+      </c>
+      <c r="D58" t="n">
+        <v>586.5476311067085</v>
+      </c>
+      <c r="E58" t="n">
+        <v>56.72607567224335</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>RVTY</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>0.004873960800547762</v>
+      </c>
+      <c r="C59" t="n">
+        <v>98.26999664306641</v>
+      </c>
+      <c r="D59" t="n">
+        <v>583.5066878729376</v>
+      </c>
+      <c r="E59" t="n">
+        <v>5.937790859933929</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>MAR</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>0.004856661685269422</v>
+      </c>
+      <c r="C60" t="n">
+        <v>295.8399963378906</v>
+      </c>
+      <c r="D60" t="n">
+        <v>581.4356516311069</v>
+      </c>
+      <c r="E60" t="n">
+        <v>1.965372021459283</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>MTD</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>0.004807149128987796</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1452.349975585938</v>
+      </c>
+      <c r="D61" t="n">
+        <v>575.5080480031157</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.3962598944313902</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>WBD</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>0.004783278036990956</v>
+      </c>
+      <c r="C62" t="n">
+        <v>23.17000007629395</v>
+      </c>
+      <c r="D62" t="n">
+        <v>572.6502199661277</v>
+      </c>
+      <c r="E62" t="n">
+        <v>24.71515831163188</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>FOX</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>0.004551799621236686</v>
+      </c>
+      <c r="C63" t="n">
+        <v>59.13999938964844</v>
+      </c>
+      <c r="D63" t="n">
+        <v>544.937809214759</v>
+      </c>
+      <c r="E63" t="n">
+        <v>9.214369544111666</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>KVUE</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>0.004264866655791828</v>
+      </c>
+      <c r="C64" t="n">
+        <v>16.63999938964844</v>
+      </c>
+      <c r="D64" t="n">
+        <v>510.586424138073</v>
+      </c>
+      <c r="E64" t="n">
+        <v>30.68428142225193</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>TECH</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>0.00410561877189093</v>
+      </c>
+      <c r="C65" t="n">
+        <v>61.52999877929688</v>
+      </c>
+      <c r="D65" t="n">
+        <v>491.5213948757646</v>
+      </c>
+      <c r="E65" t="n">
+        <v>7.988321219358578</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>KO</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0.004048119792977012</v>
+      </c>
+      <c r="C66" t="n">
+        <v>72.94999694824219</v>
+      </c>
+      <c r="D66" t="n">
+        <v>484.6376631193735</v>
+      </c>
+      <c r="E66" t="n">
+        <v>6.643422664749699</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>IDXX</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0.003994170994449389</v>
+      </c>
+      <c r="C67" t="n">
+        <v>725.9099731445312</v>
+      </c>
+      <c r="D67" t="n">
+        <v>478.1789561186853</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.6587303850466292</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>FICO</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>0.003466313932054735</v>
+      </c>
+      <c r="C68" t="n">
+        <v>1788.199951171875</v>
+      </c>
+      <c r="D68" t="n">
+        <v>414.9843308944473</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.2320681927222358</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>JNJ</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>0.003325227650296157</v>
+      </c>
+      <c r="C69" t="n">
+        <v>203.8999938964844</v>
+      </c>
+      <c r="D69" t="n">
+        <v>398.0935941113356</v>
+      </c>
+      <c r="E69" t="n">
+        <v>1.952396302245301</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>FSLR</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>0.002879760558579525</v>
+      </c>
+      <c r="C70" t="n">
+        <v>249.9100036621094</v>
+      </c>
+      <c r="D70" t="n">
+        <v>344.7626302646939</v>
+      </c>
+      <c r="E70" t="n">
+        <v>1.379547137820181</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>PODD</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>0.002716426184487038</v>
+      </c>
+      <c r="C71" t="n">
+        <v>331.1700134277344</v>
+      </c>
+      <c r="D71" t="n">
+        <v>325.2083696658406</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.981998238004134</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>NEM</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>0.001860313310324049</v>
+      </c>
+      <c r="C72" t="n">
+        <v>83.48999786376953</v>
+      </c>
+      <c r="D72" t="n">
+        <v>222.7152212613469</v>
+      </c>
+      <c r="E72" t="n">
+        <v>2.667567696249686</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>EQT</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>0.001550473905431937</v>
+      </c>
+      <c r="C73" t="n">
+        <v>57.02999877929688</v>
+      </c>
+      <c r="D73" t="n">
+        <v>185.6214955791871</v>
+      </c>
+      <c r="E73" t="n">
+        <v>3.254804481015906</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>ALL</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>0.001539220891886243</v>
+      </c>
+      <c r="C74" t="n">
+        <v>214.3200073242188</v>
+      </c>
+      <c r="D74" t="n">
+        <v>184.2742937999076</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.8598091055546733</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>MMM</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>0.001163169511834816</v>
+      </c>
+      <c r="C75" t="n">
+        <v>168.0899963378906</v>
+      </c>
+      <c r="D75" t="n">
+        <v>139.2537234212547</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.8284474177828531</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>CNC</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>0.0005752091082858414</v>
+      </c>
+      <c r="C76" t="n">
+        <v>36.5</v>
+      </c>
+      <c r="D76" t="n">
+        <v>68.86357427669429</v>
+      </c>
+      <c r="E76" t="n">
+        <v>1.886673267854638</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>EIX</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>0.0003622503055675387</v>
+      </c>
+      <c r="C77" t="n">
+        <v>58.58000183105469</v>
+      </c>
+      <c r="D77" t="n">
+        <v>43.36831678230127</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.7403263131909066</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>MNST</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>0.0001895625353687091</v>
+      </c>
+      <c r="C78" t="n">
+        <v>72.04000091552734</v>
+      </c>
+      <c r="D78" t="n">
+        <v>22.69427508431356</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.3150232481385502</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>BMY</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>0.000141264436784025</v>
+      </c>
+      <c r="C79" t="n">
+        <v>46.25</v>
+      </c>
+      <c r="D79" t="n">
+        <v>16.91206536023404</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.3656662780591144</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>IFF</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>0.0001318793545292135</v>
+      </c>
+      <c r="C80" t="n">
+        <v>67.44999694824219</v>
+      </c>
+      <c r="D80" t="n">
+        <v>15.78849082075381</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.2340769686449226</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>RL</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>9.685517648074387e-05</v>
+      </c>
+      <c r="C81" t="n">
+        <v>339.8800048828125</v>
+      </c>
+      <c r="D81" t="n">
+        <v>11.59542424413347</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.03411622948555466</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G81"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Shares</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Entry_Price</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Exit_Price</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Sale_Value</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>Transaction_Cost</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>Gain_Loss</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>WELL</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>28.33313523471959</v>
+      </c>
+      <c r="C2" t="n">
+        <v>199.9299926757812</v>
+      </c>
+      <c r="D2" t="n">
+        <v>202.3000030517578</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5731.79334444964</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>67.14982449023228</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CAH</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>27.02750673675283</v>
+      </c>
+      <c r="C3" t="n">
+        <v>209.4799957275391</v>
+      </c>
+      <c r="D3" t="n">
+        <v>211.1999969482422</v>
+      </c>
+      <c r="E3" t="n">
+        <v>5708.209340320792</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>46.48734457977662</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>COR</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>13.02716773987273</v>
+      </c>
+      <c r="C4" t="n">
+        <v>365.6799926757812</v>
+      </c>
+      <c r="D4" t="n">
+        <v>372.2200012207031</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4848.972392037733</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>85.19778833489818</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>HCA</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>8.172697697047148</v>
+      </c>
+      <c r="C5" t="n">
+        <v>491</v>
+      </c>
+      <c r="D5" t="n">
+        <v>501.0400085449219</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4094.848523963567</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>82.05395471341672</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>VTR</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>49.91614195502652</v>
+      </c>
+      <c r="C6" t="n">
+        <v>79.23999786376953</v>
+      </c>
+      <c r="D6" t="n">
+        <v>78.80000305175781</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3933.392138388066</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-21.96284349585221</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MCK</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4.062669076046815</v>
+      </c>
+      <c r="C7" t="n">
+        <v>866.030029296875</v>
+      </c>
+      <c r="D7" t="n">
+        <v>870.2100219726562</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3535.37534593433</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>16.98192698199864</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>LLY</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>3.238376742702901</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1059.699951171875</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1070.160034179688</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3465.581365657641</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>33.8736895392417</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>EXPD</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>23.01394456293329</v>
+      </c>
+      <c r="C9" t="n">
+        <v>143.2100067138672</v>
+      </c>
+      <c r="D9" t="n">
+        <v>144.2599945068359</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3319.991516229383</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>24.16436085913983</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>10.28350783947611</v>
+      </c>
+      <c r="C10" t="n">
+        <v>299.6499938964844</v>
+      </c>
+      <c r="D10" t="n">
+        <v>318.4700012207031</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3274.988754191067</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>193.5356928576016</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>3.456471808278343</v>
+      </c>
+      <c r="C11" t="n">
+        <v>839.5700073242188</v>
+      </c>
+      <c r="D11" t="n">
+        <v>840.02001953125</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2903.505515899189</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1.555454506984461</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>9.647933142923126</v>
+      </c>
+      <c r="C12" t="n">
+        <v>299.6600036621094</v>
+      </c>
+      <c r="D12" t="n">
+        <v>318.5799865722656</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3073.638411122566</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>182.5387301824358</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>DHR</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>12.02003898073451</v>
+      </c>
+      <c r="C13" t="n">
+        <v>227.3899993896484</v>
+      </c>
+      <c r="D13" t="n">
+        <v>226.9799957275391</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2728.308396491972</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>-4.928260000798673</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>EXPE</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>10.72482835382161</v>
+      </c>
+      <c r="C14" t="n">
+        <v>247.4900054931641</v>
+      </c>
+      <c r="D14" t="n">
+        <v>249.1399993896484</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2671.983729525201</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>17.69590132464828</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>CSCO</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>34.02207816173695</v>
+      </c>
+      <c r="C15" t="n">
+        <v>76.09999847412109</v>
+      </c>
+      <c r="D15" t="n">
+        <v>76.23999786376953</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2593.843166371825</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>4.763070177214558</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>WAT</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>6.286496859916102</v>
+      </c>
+      <c r="C16" t="n">
+        <v>393.989990234375</v>
+      </c>
+      <c r="D16" t="n">
+        <v>399.5400085449219</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2511.707009128504</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>34.89017268172984</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>FDS</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>8.408057680806175</v>
+      </c>
+      <c r="C17" t="n">
+        <v>277.0199890136719</v>
+      </c>
+      <c r="D17" t="n">
+        <v>271.760009765625</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2284.973837445824</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>-44.2262089174219</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>DD</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>60.19646992580901</v>
+      </c>
+      <c r="C18" t="n">
+        <v>38.54000091552734</v>
+      </c>
+      <c r="D18" t="n">
+        <v>38.47000122070312</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2315.758271527891</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>-4.213734524301799</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>UPS</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>22.41790493993123</v>
+      </c>
+      <c r="C19" t="n">
+        <v>94.66000366210938</v>
+      </c>
+      <c r="D19" t="n">
+        <v>93.55999755859375</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2097.419131448753</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>-24.65983226195749</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>EPAM</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>11.4694776359899</v>
+      </c>
+      <c r="C20" t="n">
+        <v>180.9799957275391</v>
+      </c>
+      <c r="D20" t="n">
+        <v>183.2299957275391</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2101.552338239535</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>25.80632468097747</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>AMGN</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>6.002101471457562</v>
+      </c>
+      <c r="C21" t="n">
+        <v>337.5400085449219</v>
+      </c>
+      <c r="D21" t="n">
+        <v>334.2999877929688</v>
+      </c>
+      <c r="E21" t="n">
+        <v>2006.502448640423</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>-19.44693332285078</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>LVS</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>31.25453489573897</v>
+      </c>
+      <c r="C22" t="n">
+        <v>64.30999755859375</v>
+      </c>
+      <c r="D22" t="n">
+        <v>65.66999816894531</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2052.485249374416</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>42.50618653445895</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>ISRG</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>3.533428805899726</v>
+      </c>
+      <c r="C23" t="n">
+        <v>561.6099853515625</v>
+      </c>
+      <c r="D23" t="n">
+        <v>568.47998046875</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2008.683538565595</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>24.27463864346078</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>AKAM</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>22.01197594925345</v>
+      </c>
+      <c r="C24" t="n">
+        <v>89.01000213623047</v>
+      </c>
+      <c r="D24" t="n">
+        <v>88.33999633789062</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1944.537874746786</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>-14.74815151891698</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>EW</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>22.66457084305964</v>
+      </c>
+      <c r="C25" t="n">
+        <v>85.12999725341797</v>
+      </c>
+      <c r="D25" t="n">
+        <v>84.70999908447266</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1919.915775365547</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>-9.519078254016222</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>CMI</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>3.952864785911092</v>
+      </c>
+      <c r="C26" t="n">
+        <v>472.510009765625</v>
+      </c>
+      <c r="D26" t="n">
+        <v>485.6199951171875</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1919.590178033047</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>51.82199944000149</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>ROK</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>4.804712480152092</v>
+      </c>
+      <c r="C27" t="n">
+        <v>378.7300109863281</v>
+      </c>
+      <c r="D27" t="n">
+        <v>384.3699951171875</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1846.787312535549</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>27.09850214139965</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>TMO</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>3.053851977835376</v>
+      </c>
+      <c r="C28" t="n">
+        <v>587.47998046875</v>
+      </c>
+      <c r="D28" t="n">
+        <v>586.0700073242188</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1789.771051017058</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>-4.305849276121535</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>STE</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>6.666123259013066</v>
+      </c>
+      <c r="C29" t="n">
+        <v>263.2900085449219</v>
+      </c>
+      <c r="D29" t="n">
+        <v>263.0799865722656</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1753.723617470225</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>-1.400032356827523</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>UHS</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>7.562444837680207</v>
+      </c>
+      <c r="C30" t="n">
+        <v>231.9199981689453</v>
+      </c>
+      <c r="D30" t="n">
+        <v>236.9499969482422</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1791.921281209575</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>38.03908830203136</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>HSIC</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>23.26426769253423</v>
+      </c>
+      <c r="C31" t="n">
+        <v>73.40000152587891</v>
+      </c>
+      <c r="D31" t="n">
+        <v>74.45999908447266</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1732.257351087026</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>24.66006695655778</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>FDX</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>6.309865225907285</v>
+      </c>
+      <c r="C32" t="n">
+        <v>269.4299926757812</v>
+      </c>
+      <c r="D32" t="n">
+        <v>266.9800109863281</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1684.607887334977</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>-15.45905426638978</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>EXE</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>14.61507223952759</v>
+      </c>
+      <c r="C33" t="n">
+        <v>114.9899978637695</v>
+      </c>
+      <c r="D33" t="n">
+        <v>116.5500030517578</v>
+      </c>
+      <c r="E33" t="n">
+        <v>1703.386714118602</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>22.79958851648644</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>AEP</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>13.17404895493532</v>
+      </c>
+      <c r="C34" t="n">
+        <v>120.8399963378906</v>
+      </c>
+      <c r="D34" t="n">
+        <v>122.0400009155273</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1607.760946521509</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>15.80891905193266</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>10.48558720772088</v>
+      </c>
+      <c r="C35" t="n">
+        <v>151.25</v>
+      </c>
+      <c r="D35" t="n">
+        <v>153.6000061035156</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1610.586259104873</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>24.64119393708938</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>JKHY</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>9.196072372908347</v>
+      </c>
+      <c r="C36" t="n">
+        <v>170.8000030517578</v>
+      </c>
+      <c r="D36" t="n">
+        <v>170.5800018310547</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1568.666042209217</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>-2.023147147714099</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>KDP</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>55.72822222639387</v>
+      </c>
+      <c r="C37" t="n">
+        <v>27.73999977111816</v>
+      </c>
+      <c r="D37" t="n">
+        <v>27.36000061035156</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1524.724194127944</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>-21.17667767704438</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>MRK</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>13.59923137288419</v>
+      </c>
+      <c r="C38" t="n">
+        <v>97.76000213623047</v>
+      </c>
+      <c r="D38" t="n">
+        <v>100.4000015258789</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1365.362850588353</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>35.90196252410215</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>REGN</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1.709923288585197</v>
+      </c>
+      <c r="C39" t="n">
+        <v>755.9000244140625</v>
+      </c>
+      <c r="D39" t="n">
+        <v>761.4500122070312</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1302.021108966285</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>9.490053378560788</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>CB</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>4.148055677004152</v>
+      </c>
+      <c r="C40" t="n">
+        <v>298.2900085449219</v>
+      </c>
+      <c r="D40" t="n">
+        <v>295.8099975585938</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1227.036339687509</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>-10.28722365087106</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>CTSH</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>16.0011903235469</v>
+      </c>
+      <c r="C41" t="n">
+        <v>75.98000335693359</v>
+      </c>
+      <c r="D41" t="n">
+        <v>74.91999816894531</v>
+      </c>
+      <c r="E41" t="n">
+        <v>1198.809149741079</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>-16.96134475694771</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>IQV</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>5.229080435699405</v>
+      </c>
+      <c r="C42" t="n">
+        <v>224.8999938964844</v>
+      </c>
+      <c r="D42" t="n">
+        <v>228.1799926757812</v>
+      </c>
+      <c r="E42" t="n">
+        <v>1193.171535518961</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>17.15137744593926</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>INCY</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>10.58815793136725</v>
+      </c>
+      <c r="C43" t="n">
+        <v>102.0599975585938</v>
+      </c>
+      <c r="D43" t="n">
+        <v>106.2399978637695</v>
+      </c>
+      <c r="E43" t="n">
+        <v>1124.885876009711</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>44.2585033843643</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>ABBV</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>4.562366970007153</v>
+      </c>
+      <c r="C44" t="n">
+        <v>236.2799987792969</v>
+      </c>
+      <c r="D44" t="n">
+        <v>229.5099945068359</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1047.108818224511</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>-30.88724387948309</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>DOV</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>5.523847272306242</v>
+      </c>
+      <c r="C45" t="n">
+        <v>183.5800018310547</v>
+      </c>
+      <c r="D45" t="n">
+        <v>183.0399932861328</v>
+      </c>
+      <c r="E45" t="n">
+        <v>1011.084967636558</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>-2.982924727888758</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>BIIB</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>5.767831166761293</v>
+      </c>
+      <c r="C46" t="n">
+        <v>175.3000030517578</v>
+      </c>
+      <c r="D46" t="n">
+        <v>176.8200073242188</v>
+      </c>
+      <c r="E46" t="n">
+        <v>1019.867949151589</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>8.767128016310494</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>GM</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>13.23211830410416</v>
+      </c>
+      <c r="C47" t="n">
+        <v>70.33000183105469</v>
+      </c>
+      <c r="D47" t="n">
+        <v>71</v>
+      </c>
+      <c r="E47" t="n">
+        <v>939.4803995913954</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>8.865495035017602</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>ALB</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>7.704582251068043</v>
+      </c>
+      <c r="C48" t="n">
+        <v>116.8199996948242</v>
+      </c>
+      <c r="D48" t="n">
+        <v>115.879997253418</v>
+      </c>
+      <c r="E48" t="n">
+        <v>892.8069700924976</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>-7.242326126019293</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>HIG</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>6.556915980479311</v>
+      </c>
+      <c r="C49" t="n">
+        <v>136.4499969482422</v>
+      </c>
+      <c r="D49" t="n">
+        <v>136.6399993896484</v>
+      </c>
+      <c r="E49" t="n">
+        <v>895.9369955706692</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>1.245830044386707</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>GILD</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>6.867249973173125</v>
+      </c>
+      <c r="C50" t="n">
+        <v>126.6399993896484</v>
+      </c>
+      <c r="D50" t="n">
+        <v>125.2699966430664</v>
+      </c>
+      <c r="E50" t="n">
+        <v>860.2603810864953</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>-9.408151324712549</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>CHRW</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>5.642485852260685</v>
+      </c>
+      <c r="C51" t="n">
+        <v>151.6799926757812</v>
+      </c>
+      <c r="D51" t="n">
+        <v>154.5700073242188</v>
+      </c>
+      <c r="E51" t="n">
+        <v>872.1590795107347</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>16.3068667666347</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>NUE</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>5.416558871801353</v>
+      </c>
+      <c r="C52" t="n">
+        <v>152.3500061035156</v>
+      </c>
+      <c r="D52" t="n">
+        <v>153.6499938964844</v>
+      </c>
+      <c r="E52" t="n">
+        <v>832.2542375922262</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="n">
+        <v>7.041460413238383</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>STLD</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>5.106999464619511</v>
+      </c>
+      <c r="C53" t="n">
+        <v>158.1600036621094</v>
+      </c>
+      <c r="D53" t="n">
+        <v>161.1900024414062</v>
+      </c>
+      <c r="E53" t="n">
+        <v>823.1972561702794</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" t="n">
+        <v>15.47420214366696</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>CTRA</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>29.19571912820349</v>
+      </c>
+      <c r="C54" t="n">
+        <v>25.75</v>
+      </c>
+      <c r="D54" t="n">
+        <v>26.20000076293945</v>
+      </c>
+      <c r="E54" t="n">
+        <v>764.9278634334974</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="n">
+        <v>13.13809588225752</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>JBHT</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>3.93038177703611</v>
+      </c>
+      <c r="C55" t="n">
+        <v>166.4299926757812</v>
+      </c>
+      <c r="D55" t="n">
+        <v>166.6499938964844</v>
+      </c>
+      <c r="E55" t="n">
+        <v>654.9980991539211</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.8646887887772436</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>CAT</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>1.159640332522988</v>
+      </c>
+      <c r="C56" t="n">
+        <v>550.4299926757812</v>
+      </c>
+      <c r="D56" t="n">
+        <v>559.5999755859375</v>
+      </c>
+      <c r="E56" t="n">
+        <v>648.9347017683324</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" t="n">
+        <v>10.63388203116369</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>FOXA</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>8.998992310675217</v>
+      </c>
+      <c r="C57" t="n">
+        <v>65.69000244140625</v>
+      </c>
+      <c r="D57" t="n">
+        <v>64.30000305175781</v>
+      </c>
+      <c r="E57" t="n">
+        <v>578.6352330391616</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" t="n">
+        <v>-12.50859381928944</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>VTRS</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>56.72607567224335</v>
+      </c>
+      <c r="C58" t="n">
+        <v>10.34000015258789</v>
+      </c>
+      <c r="D58" t="n">
+        <v>10.56999969482422</v>
+      </c>
+      <c r="E58" t="n">
+        <v>599.5946025441878</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" t="n">
+        <v>13.04697143747921</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>RVTY</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>5.937790859933929</v>
+      </c>
+      <c r="C59" t="n">
+        <v>98.26999664306641</v>
+      </c>
+      <c r="D59" t="n">
+        <v>100.5800018310547</v>
+      </c>
+      <c r="E59" t="n">
+        <v>597.2230155645743</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" t="n">
+        <v>13.71632769163671</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>MAR</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>1.965372021459283</v>
+      </c>
+      <c r="C60" t="n">
+        <v>295.8399963378906</v>
+      </c>
+      <c r="D60" t="n">
+        <v>296.2300109863281</v>
+      </c>
+      <c r="E60" t="n">
+        <v>582.2021755091052</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.7665238779983383</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>MTD</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>0.3962598944313902</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1452.349975585938</v>
+      </c>
+      <c r="D61" t="n">
+        <v>1470.140014648438</v>
+      </c>
+      <c r="E61" t="n">
+        <v>582.5575270039523</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="n">
+        <v>7.049479000836527</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>WBD</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>24.71515831163188</v>
+      </c>
+      <c r="C62" t="n">
+        <v>23.17000007629395</v>
+      </c>
+      <c r="D62" t="n">
+        <v>22.86000061035156</v>
+      </c>
+      <c r="E62" t="n">
+        <v>564.9885340888403</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" t="n">
+        <v>-7.661685877287368</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>FOX</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>9.214369544111666</v>
+      </c>
+      <c r="C63" t="n">
+        <v>59.13999938964844</v>
+      </c>
+      <c r="D63" t="n">
+        <v>57.70999908447266</v>
+      </c>
+      <c r="E63" t="n">
+        <v>531.7612579546769</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0</v>
+      </c>
+      <c r="G63" t="n">
+        <v>-13.17655126008208</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>KVUE</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>30.68428142225193</v>
+      </c>
+      <c r="C64" t="n">
+        <v>16.63999938964844</v>
+      </c>
+      <c r="D64" t="n">
+        <v>16.76000022888184</v>
+      </c>
+      <c r="E64" t="n">
+        <v>514.268563660017</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G64" t="n">
+        <v>3.682139521944009</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>TECH</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>7.988321219358578</v>
+      </c>
+      <c r="C65" t="n">
+        <v>61.52999877929688</v>
+      </c>
+      <c r="D65" t="n">
+        <v>63.4900016784668</v>
+      </c>
+      <c r="E65" t="n">
+        <v>507.178527625208</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0</v>
+      </c>
+      <c r="G65" t="n">
+        <v>15.65713274944341</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>KO</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>6.643422664749699</v>
+      </c>
+      <c r="C66" t="n">
+        <v>72.94999694824219</v>
+      </c>
+      <c r="D66" t="n">
+        <v>72.58999633789062</v>
+      </c>
+      <c r="E66" t="n">
+        <v>482.2460269052402</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" t="n">
+        <v>-2.391636214133314</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>IDXX</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0.6587303850466292</v>
+      </c>
+      <c r="C67" t="n">
+        <v>725.9099731445312</v>
+      </c>
+      <c r="D67" t="n">
+        <v>752.1400146484375</v>
+      </c>
+      <c r="E67" t="n">
+        <v>495.4574814583426</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0</v>
+      </c>
+      <c r="G67" t="n">
+        <v>17.27852533965722</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>FICO</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>0.2320681927222358</v>
+      </c>
+      <c r="C68" t="n">
+        <v>1788.199951171875</v>
+      </c>
+      <c r="D68" t="n">
+        <v>1748.25</v>
+      </c>
+      <c r="E68" t="n">
+        <v>405.7132179266487</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" t="n">
+        <v>-9.271112967798558</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>JNJ</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>1.952396302245301</v>
+      </c>
+      <c r="C69" t="n">
+        <v>203.8999938964844</v>
+      </c>
+      <c r="D69" t="n">
+        <v>206.0500030517578</v>
+      </c>
+      <c r="E69" t="n">
+        <v>402.291264035885</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0</v>
+      </c>
+      <c r="G69" t="n">
+        <v>4.197669924549416</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>FSLR</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>1.379547137820181</v>
+      </c>
+      <c r="C70" t="n">
+        <v>249.9100036621094</v>
+      </c>
+      <c r="D70" t="n">
+        <v>259.8500061035156</v>
+      </c>
+      <c r="E70" t="n">
+        <v>358.4753321826615</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" t="n">
+        <v>13.71270191796759</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>PODD</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>0.981998238004134</v>
+      </c>
+      <c r="C71" t="n">
+        <v>331.1700134277344</v>
+      </c>
+      <c r="D71" t="n">
+        <v>337.5299987792969</v>
+      </c>
+      <c r="E71" t="n">
+        <v>331.453864074807</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" t="n">
+        <v>6.245494408966465</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>NEM</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>2.667567696249686</v>
+      </c>
+      <c r="C72" t="n">
+        <v>83.48999786376953</v>
+      </c>
+      <c r="D72" t="n">
+        <v>86.52999877929688</v>
+      </c>
+      <c r="E72" t="n">
+        <v>230.8246295001771</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0</v>
+      </c>
+      <c r="G72" t="n">
+        <v>8.109408238830213</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>EQT</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>3.254804481015906</v>
+      </c>
+      <c r="C73" t="n">
+        <v>57.02999877929688</v>
+      </c>
+      <c r="D73" t="n">
+        <v>57.54000091552734</v>
+      </c>
+      <c r="E73" t="n">
+        <v>187.2814528175177</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0</v>
+      </c>
+      <c r="G73" t="n">
+        <v>1.659957238330634</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>ALL</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>0.8598091055546733</v>
+      </c>
+      <c r="C74" t="n">
+        <v>214.3200073242188</v>
+      </c>
+      <c r="D74" t="n">
+        <v>212.3699951171875</v>
+      </c>
+      <c r="E74" t="n">
+        <v>182.5976555483593</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" t="n">
+        <v>-1.676638251548241</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>MMM</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>0.8284474177828531</v>
+      </c>
+      <c r="C75" t="n">
+        <v>168.0899963378906</v>
+      </c>
+      <c r="D75" t="n">
+        <v>169.5599975585938</v>
+      </c>
+      <c r="E75" t="n">
+        <v>140.4715421366839</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0</v>
+      </c>
+      <c r="G75" t="n">
+        <v>1.217818715429132</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>CNC</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>1.886673267854638</v>
+      </c>
+      <c r="C76" t="n">
+        <v>36.5</v>
+      </c>
+      <c r="D76" t="n">
+        <v>38.16999816894531</v>
+      </c>
+      <c r="E76" t="n">
+        <v>72.01431517940961</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G76" t="n">
+        <v>3.150740902715313</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>EIX</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>0.7403263131909066</v>
+      </c>
+      <c r="C77" t="n">
+        <v>58.58000183105469</v>
+      </c>
+      <c r="D77" t="n">
+        <v>59.18000030517578</v>
+      </c>
+      <c r="E77" t="n">
+        <v>43.81251144056751</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0.444194658266241</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>MNST</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>0.3150232481385502</v>
+      </c>
+      <c r="C78" t="n">
+        <v>72.04000091552734</v>
+      </c>
+      <c r="D78" t="n">
+        <v>73.23999786376953</v>
+      </c>
+      <c r="E78" t="n">
+        <v>23.07230202070516</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0.3780269363916027</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>BMY</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>0.3656662780591144</v>
+      </c>
+      <c r="C79" t="n">
+        <v>46.25</v>
+      </c>
+      <c r="D79" t="n">
+        <v>47.7599983215332</v>
+      </c>
+      <c r="E79" t="n">
+        <v>17.4642208263446</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0</v>
+      </c>
+      <c r="G79" t="n">
+        <v>0.5521554661105554</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>IFF</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>0.2340769686449226</v>
+      </c>
+      <c r="C80" t="n">
+        <v>67.44999694824219</v>
+      </c>
+      <c r="D80" t="n">
+        <v>67.44999694824219</v>
+      </c>
+      <c r="E80" t="n">
+        <v>15.78849082075381</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>RL</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>0.03411622948555466</v>
+      </c>
+      <c r="C81" t="n">
+        <v>339.8800048828125</v>
+      </c>
+      <c r="D81" t="n">
+        <v>349.9800109863281</v>
+      </c>
+      <c r="E81" t="n">
+        <v>11.93999837016651</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0</v>
+      </c>
+      <c r="G81" t="n">
+        <v>0.3445741260330433</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>